<commit_message>
Api: add quiz and answer request api
</commit_message>
<xml_diff>
--- a/lib/samples/assets/csv/categories.xlsx
+++ b/lib/samples/assets/csv/categories.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="123">
   <si>
     <t>code</t>
   </si>
@@ -297,6 +297,9 @@
     <t>your_safety_safety_planning.png</t>
   </si>
   <si>
+    <t>right_and_your_safety.mp3</t>
+  </si>
+  <si>
     <t>sa_001_1</t>
   </si>
   <si>
@@ -306,6 +309,9 @@
     <t>violence_on_women.png</t>
   </si>
   <si>
+    <t>violence_on_women.mp3</t>
+  </si>
+  <si>
     <t>sa_001_2</t>
   </si>
   <si>
@@ -315,6 +321,9 @@
     <t>harassment.png</t>
   </si>
   <si>
+    <t>harassment.mp3</t>
+  </si>
+  <si>
     <t>sa_001_3</t>
   </si>
   <si>
@@ -324,12 +333,18 @@
     <t>your_health.png</t>
   </si>
   <si>
+    <t>your_health.mp3</t>
+  </si>
+  <si>
     <t>sa_001_4</t>
   </si>
   <si>
     <t>ស្វែងយល់អំពីការកេងប្រវញ្ច័​និងការជួញដូរ</t>
   </si>
   <si>
+    <t>understand_exploitation_and_human_traficking.mp3</t>
+  </si>
+  <si>
     <t>sa_001_5</t>
   </si>
   <si>
@@ -346,6 +361,9 @@
   </si>
   <si>
     <t>safety_planning_tips.png</t>
+  </si>
+  <si>
+    <t>my_body_my_choice_safety_planning_tips.mp3</t>
   </si>
   <si>
     <t>sa_002_1</t>
@@ -1051,6 +1069,7 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="36.0"/>
     <col customWidth="1" min="3" max="3" width="21.86"/>
+    <col customWidth="1" min="4" max="4" width="45.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1086,16 +1105,22 @@
       <c r="C2" s="3" t="s">
         <v>86</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>84</v>
@@ -1103,13 +1128,16 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>84</v>
@@ -1117,13 +1145,16 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>84</v>
@@ -1131,10 +1162,13 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>97</v>
+        <v>101</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>84</v>
@@ -1142,13 +1176,13 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>84</v>
@@ -1156,77 +1190,80 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>103</v>
+        <v>108</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>82</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="G13" s="3" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Category: update missing image
</commit_message>
<xml_diff>
--- a/lib/samples/assets/csv/categories.xlsx
+++ b/lib/samples/assets/csv/categories.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="128">
   <si>
     <t>code</t>
   </si>
@@ -219,6 +219,9 @@
     <t>វប្បធម៌ និងការរស់នៅ</t>
   </si>
   <si>
+    <t>culture_and_living.png</t>
+  </si>
+  <si>
     <t>migration_calture_and_living.mp3</t>
   </si>
   <si>
@@ -228,6 +231,9 @@
     <t>គន្លឹះក្នុងការសន្សំប្រាក់</t>
   </si>
   <si>
+    <t>money_saving_tip.png</t>
+  </si>
+  <si>
     <t>migration_saving_tip.mp3</t>
   </si>
   <si>
@@ -255,6 +261,9 @@
     <t>រៀបចំផែនការរបស់អ្នក</t>
   </si>
   <si>
+    <t>coming_home_make_your_plan.png</t>
+  </si>
+  <si>
     <t>coming_home_prepare_plan.mp3</t>
   </si>
   <si>
@@ -342,6 +351,9 @@
     <t>ស្វែងយល់អំពីការកេងប្រវញ្ច័​និងការជួញដូរ</t>
   </si>
   <si>
+    <t>understand_exploitation_and_human_traficking.png</t>
+  </si>
+  <si>
     <t>understand_exploitation_and_human_traficking.mp3</t>
   </si>
   <si>
@@ -388,6 +400,9 @@
   </si>
   <si>
     <t>ចំនុចដែលគួរដឹង</t>
+  </si>
+  <si>
+    <t>thing_need_to_know.png</t>
   </si>
   <si>
     <t>sa_002_4</t>
@@ -409,7 +424,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -421,9 +436,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-    </font>
-    <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -432,7 +444,9 @@
       <color rgb="FF212529"/>
       <name val="Nunito"/>
     </font>
-    <font/>
+    <font>
+      <name val="Arial"/>
+    </font>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -458,33 +472,59 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -711,8 +751,7 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="46.71"/>
     <col customWidth="1" min="3" max="3" width="51.57"/>
-    <col customWidth="1" min="4" max="4" width="21.71"/>
-    <col customWidth="1" min="8" max="9" width="28.0"/>
+    <col customWidth="1" min="4" max="4" width="39.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -737,319 +776,415 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="C14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="I15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="B16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="B17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="A18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G19" s="3" t="b">
+      <c r="A19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="7" t="b">
         <v>1</v>
       </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId2"/>
@@ -1063,13 +1198,16 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="36.0"/>
-    <col customWidth="1" min="3" max="3" width="21.86"/>
-    <col customWidth="1" min="4" max="4" width="45.86"/>
+    <col customWidth="1" min="3" max="3" width="29.14"/>
+    <col customWidth="1" min="4" max="4" width="45.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1096,196 +1234,216 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G13" s="3" t="b">
+      <c r="C13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15">
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16">
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17">
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19">
-      <c r="B19" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
category: add rich text and content for description
</commit_message>
<xml_diff>
--- a/lib/samples/assets/csv/categories.xlsx
+++ b/lib/samples/assets/csv/categories.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="149">
   <si>
     <t>code</t>
   </si>
@@ -99,6 +99,9 @@
     <t>passport.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;លិខិតឆ្លងដែនត្រូវការជាចាំបាច់សម្រាប់ការឆ្លងដែនរបស់អ្នក។ អ្នកអាចស្វែងរកពីរបៀបធ្វើលិខិតឆ្លងដែនពីអាជ្ញាធរមូលដ្ឋាន ឬក្រុមហ៊ុនដែលអ្នកបានចុះឈ្មោះទៅធ្វើការជាមួយ។&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>de_001_2</t>
   </si>
   <si>
@@ -111,6 +114,9 @@
     <t>visa.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;ទិដ្ឋាការជួយអ្នកឱ្យអ្នករស់នៅ ឬស្នាក់នៅប្រទេសគោលដៅ ដោយមានឯកសារគ្រប់គ្រាន់។ ទិដ្ឋាការអាចមានច្រើនប្រភេទខុសគ្នាពីប្រទេសមួយទៅប្រទេសមួយ។ ទិដ្ឋាការអាចមានដូចជា ទិដ្ឋាការសម្រាប់ដំណើរកម្សាន្ត ទិដ្ឋាការសម្រាប់ស្នាក់នៅរយៈពេលយូរ និងទិដ្ឋាការសម្រាប់ធ្វើការជាដើម។ &lt;/div&gt;</t>
+  </si>
+  <si>
     <t>de_001_3</t>
   </si>
   <si>
@@ -123,6 +129,12 @@
     <t>work_permit.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;
+  &lt;h2&gt;៣. ប័ណ្ណការងារ&lt;/h2&gt;
+  &lt;div&gt;ប័ណ្ណការងារបញ្ជាក់ពីសិទ្ធិរបស់អ្នកក្នុងការធ្វើការងារប្រទេសគោលដៅ។ អ្នកអាចធ្វើប័ណ្ណការងារនេះមុនពេលអ្នកចាកចេញ ឬអាចធ្វើនៅពេលដែលអ្នកទៅដល់ប្រទេសគោលដៅ។&lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>de_001_4</t>
   </si>
   <si>
@@ -135,6 +147,9 @@
     <t>transportation.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;ស្គាល់ពីប្រទេសគោលដៅរបស់អ្នក និងប្រភេទមធ្យោបាយដែលអ្នកត្រូវប្រើដើម្បីទៅដល់ប្រទេសគោលដៅ&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>de_001_5</t>
   </si>
   <si>
@@ -147,6 +162,9 @@
     <t>contact_with_home.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;វាជាការសំខាន់ណាស់ដែលអ្នកមានលេខទូរស័ព្ទទំនាក់ទំនង និងមធ្យោបាយផ្សេងៗក្នុងការទំនាក់ទំនងអ្នកផ្ទះ ឬមិត្តជិតស្និទ្ធរបស់អ្នក ដែលអាចឱ្យអ្នកផ្តល់ដំណឹងជាទៀងទាត់ពីដំណើររបស់អ្នក។ &lt;/div&gt;</t>
+  </si>
+  <si>
     <t>de_001_6</t>
   </si>
   <si>
@@ -159,6 +177,9 @@
     <t>contact_address.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;វាជាការសំខាន់ដែលអ្នកស្គាល់ពីអាស័យដ្ឋាន និងលេខទូរស័ព្ទទំនាក់ទំនងកន្លែងធ្វើការ ឬ/នឹង កន្លែងស្នាក់នៅដើម្បីងាយស្រួលក្នុងការស្វែងរកការគាំទ្រនៅពេលចាំបាច់។&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>de_002</t>
   </si>
   <si>
@@ -189,6 +210,78 @@
     <t>migration_journey_start.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 120px;'&gt;អ្នកអត្ថាធិប្បាយ៖&lt;/div&gt;
+    &lt;div style='flex: 1'&gt;
+      សួស្តីបងប្អូនដែលជា អ្នកគំាទ្រអ៊ែប (Fan App) """"ដំណើរឆ្លងដែនរបស់ខ្ញុំ។ យើងសង្ឃឹមថាមកដល់ពេលនេះបងប្អូនបានរៀបចំឯកសារពាក់ព័ន្ធរួចរាល់ និងត្រៀមសម្រាប់ការចេញដំណើរនាពេលដ៏ខ្លីខាងមុខនេះ។  ការធ្វើដំណើរ និងឆ្លងដែន គឺជាផ្នែកសំខាន់មួយនៅក្នុងដំណើរចំណាកស្រុក។
+      &lt;p&gt;សូមស្តាប់នូវការសន្ទនាខាងក្រោមនេះ អំពីបទពិសោធឆ្លងដែនរបស់កុលាបដើម្បីស្វែងរកការងារធ្វើនៅក្រៅប្រទេស។&lt;/p&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;សួស្តី កុលាប! សុខសប្បាយជាទេ?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;សួស្តី ម៉ាលីស! អរគុណច្រើន ខ្ញុំសុខសប្បាយជាធម្មតាទេ។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ខ្ញុំបានដឹងថាកុលាបធ្លាប់មានបទពិសោធចំណាកស្រុកទៅធ្វើការនៅក្រៅប្រទេស។ និយាយចឹងកុលាបទៅធ្វើការនៅប្រទេសណាដែរ? ទៅតាំងពីពេលណា? ហើយបទពិសោធរបស់កុលាបយ៉ាងម៉េចដែរពេលឆ្លងដែន?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;
+    &lt;div style='flex: 1'&gt;
+      &lt;div&gt;ខ្ញុំទៅធ្វើការនៅប្រទេសថៃ ប្រហែលជាងពីរឆ្នាំហើយ ខ្ញុំទើបមកស្រុកវិញបានប្រមាណជាងពីរអាទិត្យហ្នឹង។&lt;/div&gt;
+      &lt;p&gt;ហូ៎ ពេលបួនប្រាំថ្ងៃមុនពេលចេញដំណើរ ខ្ញុំបានសួរបងស្រីជីដូនមួយខ្ញុំដែលធ្លាប់ទៅធ្វើការនៅថៃ និងស្វែងយល់ព័ត៌មានបន្ថែមពីអ្វីដែលត្រូវការសម្រាប់ឆ្លងដែន តាមរយៈហេ្វសបុកផ្លូវការរបស់ក្រសួង និងអង្គការសង្គមស៊ីវិលមានការងារពាក់ព័ន្ធចំណាកស្រុក ស្តាប់វិទ្យុ និងខិតបណ្ណ័ផ្សព្វផ្សាយទាក់ទងនឹងចំណាកស្រុកនានា។&lt;/p&gt;
+      &lt;p&gt;ម៉ាលីសឯងចង់ទៅធ្វើការនៅប្រទេសគេមែនទេ? អញ្ចឹងម៉ាលីសត្រូវតែមានលិខិតឆ្លងដែនទិដ្ឋាការ(វីសា) និងឯកសារការងារ ឬប័ណ្ណការងារ ទើបគេអនុញ្ញាត្តិឲ្យយើងចូលប្រទេសគេដើម្បីធ្វើការ វាគឺជាតម្រូវការចំាបាច់។ កាលនោះ ខ្ញុំបានរៀបចំទុកដាក់លិខិតឆ្លងដែន ឯកសារសំខាន់ៗ លុយកាក់ និងរបស់របរប្រើប្រាស់ចាំបាច់ ដូចជាសំឡីអនាម័យ ប្រេងកូឡា ឬប្រេងខ្យល់នៅក្នុងកាបូបស្ពាយជាប់ខ្លួនដើម្បីងាយស្រួលរកពេលត្រូវការបន្ទាន់។ ខ្ញុំមិនដាក់នៅក្នុងកាតាបដាក់ខោអាវ និងគ្រឿងប្រើប្រាស់ទូទៅនោះទេ ព្រោះពេលធ្វើដំណើរកាតាបនោះមិននៅក្បែរយើងទេ។&lt;/p&gt;
+      &lt;p&gt;នៅពេលដែលយើងធ្វើដំណើរដល់ព្រំដែន យើងត្រូវបំពេញលិខិតចេញពីខាងប្រទេសយើង និងលិខិតចូលទៅខាងប្រទេសគេ។ លិខិតហ្នឹង គឹយើងត្រូវបំពេញព័ត៌មានឲ្យបានត្រឹមត្រូវ ដូចជាឈ្មោះបុគ្គល ឬឈ្មោះទីកន្លែង និងលេខទូរសព្ទ័ដែលយើងត្រូវទៅក្នុងប្រទេសថៃ។&lt;/p&gt;
+      &lt;p&gt;តាមខ្ញុំដឹង នៅពេលយើងចូលទៅប្រទេសណាក៏ដោយ ក៏ត្រូវបំពេញលិខិតចូលដែរ វាជាលក្ខខណ្ឌមិនអាចខ្វះបាន ទោះជិះឡាន ឬយន្តហោះ។&lt;/p&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ហូ៎ អីចឹងផង! ខ្ញុំមិនដែលដឹងសោះ។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ម៉ាលីសដឹងទេ  ចំពោះបទពិសោធន៍ខ្ញុំ ខ្ញុំគិតថាសំខាន់ខ្លាំងណាស់ដែលយើងធ្វើដំណើរជាមួយអ្នកដែលយើងស្គាល់ច្បាស់បំផុត អាចជាបងប្អូន ពូមីង ឬអ្នកនៅក្នុងភូមិដែលយើងស្គាល់ប្រវត្តិរបស់គេត្រឹមត្រូវ ព្រោះថានាំឲ្យខ្ញុំមានភាពកក់ក្តៅ នៅពេលមានអ្នករួមដំណើរដែលអាចជឿទុកចិត្តបាន។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ពិតមែនហើយ ពេលទៅជាមួយអ្នកស្គាល់ និងជឿទុកចិត្ត គឺអាចជួយគ្នាបាន។ ចុះពេលកុលាបធ្វើដំណើរយូរទេពីភូមិយើងទៅដល់ទល់ដែន ប្រហែលជាប៉ុន្មានម៉ោង? ជិះទៅអស់លុយប្រហែលប៉ុន្មាន?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;
+      ជិះពីភូមិយើង (ស្រុកបរសេដ្ឋ ខេត្តកំពង់ស្ពី) ទៅដល់ព្រំដែនឡែមដែលខ្ញុំឆ្លងហ្នឹង ប្រហែលជាង ៥ ទៅ ៦ ម៉ោង ព្រោះយើងមានឈប់ខ្លះ ចូលបន្ទប់ទឹក និងញាំអាហារ។  ពីភូមិទៅដល់ព្រំដែនម្នាក់អស់ប្រហែលជាង ៤ ម៉ឺនរៀល ហើយពីព្រំដែនទៅដល់គោលដៅ ជិះប្រហែលជាងពីរម៉ោងទៀត និងអស់ថ្លៃជិះចន្លោះពី ១៥០បាត ទៅ ២០០ បាត។ តាមបទពិសោធខ្ញុំ យើងគួរតែទាក់ទងឲ្យដឹងឡានណា ចេញម៉ោងប៉ុន្មាន? ចេញដំណើរពីទីតាំងណា? តើឡានហ្នឹងទៅដល់ទល់ដែនតែម្តង ឬយ៉ាងណា?
+      &lt;p&gt;បើយើងទៅជាក្រុម យើងគួរទាក់ទងគ្នាកំណត់ម៉ោងពេលចេញដំណើរឲ្យបានច្បាស់ដូចគ្នា យើងគួរតែដឹងពីទីតាំងឡានចេញដំណើរ និងគោលដៅដែលឡាននឹងឈប់ផងដែរ។&lt;/p&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;អូ៎! ល្អមែនទែន។ ខ្ញុំសុំសួរបញ្ជាក់បន្ថែម អំពីការធ្វើដំណើរពីប្រទេសយើងទៅប្រទេសគេ តើយើងត្រូវធ្វើអ្វីខ្លះ?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;អូ៎ ម៉ាលីស មុននឹងទៅដល់ទល់ដែន ខ្ញុំប្រាប់បទពិសោធសំខាន់មួយទៀតដល់ម៉ាលីសឯង។ វាពិតជាសំខាន់ណាស់! យើងត្រូវប្រាប់ពុកម៉ែ និងបងប្អូនជិតស្និត អំពីរយៈពេលនៃការធ្វើដំណើររបស់យើង ប្រហែលជាចំណាយអស់ប៉ុន្មានម៉ោង? ទៅដល់ព្រំដែនប្រហែលម៉ោងប៉ុន្មាន? ហើយឆ្លងពីព្រំដែនទៅដល់ទីកន្លែងដែលយើងត្រូវទៅចំណាយអស់ប្រហែលប៉ុន្មានម៉ោង? អូ៎មួយទៀត លេខទូរស័ព្ទទំនាក់ទំនងរបស់សាច់ញាត្តិជិតស្និតរបស់យើងក៏គួរចំា ឬកត់ត្រាទុក ដែលយើងអាចរកបានភ្លាមៗផងដែរ ពេលយើងជួបបញ្ហាបន្ទាន់ ឬពេលត្រូវការប្រើចាំបាច់។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;អរគុណសម្រាប់ការចែករំលែកបទពិសោធក្នុងការធ្វើដំណើរ។ ស្តាប់មើលទៅ គឺសំខាន់ណាស់! ចុះពេលទៅដល់ទល់ដែន កុលាបឯងមានបទពិសោធម៉េចដែរ?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;នៅច្រកទល់ដែន គឺមានសកម្មភាពចេញចូលជាហូរហែរ មានការដឹកជញ្ជូនទំនិញ និងមនុស្សឆ្លងកាត់។ ហើយការឆ្លងកាត់ទាំងនោះ មិនមែនចេញចូលស្រេចតែចិត្តនោះទេ ម៉ាលីសអើយ សុទ្ធតែឆ្លងកាត់ការត្រួតពិនិត្យពីខាងប្រទេសយើង បោះត្រាចេញពីខាងមន្ត្រីប៉ូលីសប្រចំាការងារព្រំដែន។ យើងត្រូវរង់ចាំរហូតដល់វេនរបស់យើង ប្រសិនបើមានមនុស្សចេញច្រើន។ ពេលខ្លះ ប៉ូលីសមើលការងារព្រំដែន ក៏សួរយើងមួយ ឬពីរសំនួរផងដែរ តើយើងទៅប្រទេសគេធ្វើអ្វី? ស្នាក់នៅកន្លែងណា?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;អូ៎ គេសួរយើងពីកន្លែងដែលស្នាក់នៅដែរមែនទេ? ហើយគេសួរធ្វើអី?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ពិតប្រាកដណាស់ ការដឹងព័ត៌មានកន្លែងស្នាក់នៅរបស់យើងនៅប្រទេសគោលដៅ គឺសំខាន់ណាស់។ នៅពេលយើងជួបប្រទះបញ្ហាអ្វី គេអាចដឹងពីទីកន្លែងត្រូវរកយើង។ ហើយទីតាំងស្នាក់នៅ និងអាស័យដ្ឋានកន្លែងធ្វើការនៅប្រទេសគោលដៅ ខ្ញុំក៏បានប្រាប់ទៅពុកម៉ែ និងសាច់ញាត្តិរបស់ខ្ញុំអោយបានដឹងដែរ។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ចុះកាលពេលកុលាបឯងឆ្លងដែន កុលាបដាក់ទីតាំងនៅណាដែរ?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;កាលណុង ខ្ញុំដាក់ទីតាំងស្នាក់នៅជាមួយនឹងបងប្អូនជីដូនមួយខ្ញុំ ដែលគាត់ធ្វើការ និងរស់នៅប្រទេសថៃ ដោយសារគាត់មានទីតាំងជាក់លាក់។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;អរគុណចំពោះការចែករំលែកនូវបទពិសោធ ខ្ញុំបានដឹងច្រើនពីអ្វីដែលកុលាប បានធ្វើដើម្បីឆ្លងដែន។&lt;/div&gt;
+  &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>de_002_2</t>
   </si>
   <si>
@@ -201,6 +294,16 @@
     <t>migration_understanding_your_contract.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;
+  &lt;div&gt;កិច្ចសន្យាការងារ គឺជាឯកសារស្នូលប្រាប់អ្នកអំពីលក្ខខ័ណ្ឌ អត្ថប្រយោជន៍ និងសិទ្ធិដែលអ្នកទទួលបាន។ មុននឹងចុះកិច្ចសន្យាការងារ ជាការសំខាន់ណាស់ដែលអ្នកគួរពិចារណានូវចំណុចមួយចំនួនដូចជា៖&lt;/div&gt;
+  &lt;ul&gt;
+    &lt;li&gt;ជាភាសាដែលអ្នកអាចយល់ពីលក្ខខណ្ឌនៃការងារ រួមទាំងប្រាក់ទទួលបាន អត្ថប្រយោជន៍ផ្សេងៗ ម៉ោងការងារ ថ្ងៃឈប់សម្រាកប្រចាំឆ្នាំ ថ្ងៃឈប់សម្រាកបុណ្យជាតិរបស់ប្រទេសគោលដៅ និងថ្ងៃឈប់សម្រាកពេលឈឺ។&lt;/li&gt;
+    &lt;li&gt;ស្ថានភាពការងារដែលមានសុវត្ថិភាព ជាមួយនឹងការការពារសុខភាព និងសន្តិសុខ។&lt;/li&gt;
+  &lt;/ul&gt;
+  &lt;div&gt;លើសពីនេះ កិច្ចសន្យាការងារ គឺវាសំខាន់ណាស់ ពីព្រោះវាជាឯកសារស្របច្បាប់ដែលសរសេរអំពីភារៈកិច្ច និងកាតព្វកិច្ចរបស់ភាគីនិយោជករបស់អ្នក និងអ្នកជាពលករ។ ត្រូវប្រាកដថា អ្នកបានទទួលកិច្ចសន្យាមួយច្បាប់ ព្រមទំាងអ្នកយល់ច្បាស់ពីខ្លឹមសារនៃកិច្ចសន្យានេះ។ កិច្ចសន្យាត្រូវមានចែងអំពី៖ ឈ្មោះរបស់អ្នក អាស័ន្នដ្ឋានកន្លែងធ្វើការ ឈ្មោះនិយោជក ភារៈកិច្ចរបស់អ្នក ប្រាក់ខែ និងអត្ថប្រយោជន៍របស់អ្នក ម៉ោងធ្វើការ (មិនលើស១២ម៉ោងក្នុងមួយថ្ងៃ រួមទំាងម៉ោងបន្ថែម) វិធីគណនាប្រាក់ឈ្នួលធ្វើការបន្ថែមម៉ោង សិទ្ធឈប់សំរាក ការកាត់ប្រាក់ឈ្នួលណាមួយដែលត្រូវធ្វើ និងការលំអិតអំពីការបញ្ចប់កិច្ចសន្យា។&lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>de_002_3</t>
   </si>
   <si>
@@ -213,6 +316,17 @@
     <t>migration_worker_right.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;
+  &lt;div&gt;ទោះបីជាស្ថានភាពចំណាកស្រុករបស់អ្នកយ៉ាងណាក៏ដោយ អ្នកត្រូវតែទទួលបានសិទ្ធិ និងការគាំពារពេញលេញដូចខាងក្រោម៖&lt;/div&gt;
+  &lt;ul&gt;
+    &lt;li&gt;សេរីភាពរក្សាអត្តសញ្ញាណរបស់ខ្លួន និងឯកសារសំខាន់ៗផ្សេងៗ&lt;/li&gt;
+    &lt;li&gt;សេរីភាពចូលរួមក្នុងសមាគមន៍ដូចជា សហជីព និងសមាគមន៍កម្មករ&lt;/li&gt;
+    &lt;li&gt;សេរីភាពរួចផុតពីអំពើហិង្សា និងការបៀតបៀនផ្សេងៗ រួមទាំងការបៀតបៀនផ្លូវភេទទំាងក្នុង និងក្រៅកន្លែងការងារ&lt;/li&gt;
+    &lt;li&gt;សិទ្ធិតវ៉ា និងដាក់ពាក្យបណ្តឹងពីបញ្ហានៅកន្លែងការងារ&lt;/li&gt;
+  &lt;/ul&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>de_002_4</t>
   </si>
   <si>
@@ -225,6 +339,23 @@
     <t>migration_calture_and_living.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;
+  &lt;div&gt;ជារឿងសំខាន់ណាស់ដែលយើងគួរស្វែងយល់ពីវប្បធម៌ក៏ដូចជារបៀបរបបរស់នៅក្នុងប្រទេសគោលដៅ។តោះមកស្តាប់ការសន្ទនារវាងធីតា និងរស្មី។&lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 60px;'&gt;ធីតា៖&lt;/div&gt;&lt;div style='flex: 1'&gt;រស្មីមកដល់ស្រុកវិញពីកាលណានឹង? ខ្ញុំកំពុងតែមានគម្រោងទៅក្រៅប្រទេសដើម្បីបានការងារសមរម្យមួយ និងមានប្រាក់ចំណូល។ ចឹង! តើរស្មីអាចប្រាប់ខ្ញុំបានខ្លះទេពីរបៀបរបបរស់នៅក្រៅពីស្រុកយើង?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 60px;'&gt;រស្មី៖&lt;/div&gt;&lt;div style='flex: 1'&gt;តាមបទពិសោធន៌របស់ខ្ញុំសំខាន់មែនទែន! បើយើងដឹងថាស្រុកគេនឹងរបៀបរបបរស់នៅបែបម៉េច? គេគោរពសាសនាអ្វីខ្លះ? ពេលទំនេរជាទូទៅគេធ្វើអ្វី? គេទៅដើរលេងនៅកន្លែងណា? គេបរិភោគអាហារបែបណា? សំខាន់ជាងនេះទៀតគេរាក់ទាក់គ្នាបែបណា?​ និងភាសាគន្លឹះសំរាប់ទំនាក់ទំនងមួយចំនួន? ឧទាហរណ៌ នៅប្រទេសម៉ាឡេស៊ី ភាគច្រើនគោរពសាសនាអ៊ីស្លាម ដូចនេះគេអត់ញាំសាច់ជ្រូក ហើយគេតែងតែទៅព្រះវិហារជារៀងរាល់ថ្ងៃសុក្រ ហើយគេស្វាគមន៌គ្នាដោយការនិយាយថាអាសាឡាំវ៉ាលីគុម។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 60px;'&gt;ធីតា៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ធ្វើម៉េចទៅទើបខ្ញុំដឹង បើខ្ញុំអត់ដែលទៅនៅនឹងផង?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 60px;'&gt;រស្មី៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ធ្វើដូចអ្វីដែលធីតាកំពុងមានចម្ងល់សួរមកខ្ញុំអញ្ចឹង! យើងអាចសួរអ្នកដែលធ្លាប់ទៅប្រទេសដែលយើងចង់ទៅនោះ ហើយពេលទៅដល់ធីតាអាចសាកសួរអ្នកនៅទីនោះបន្ថែមទៀត រឺក៏អាចសង្កេតមើលពីសកម្មភាពរស់នៅប្រចាំថ្ងៃរបស់អ្នកនៅទីនោះ។ បើទៅតាមក្រុមហ៊ុនអ្នកអាចសាកសួរពត៌មានពីបុគ្គលិកក្រុមហ៊ុនក៏បានដែរ។&lt;/div&gt;
+  &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>de_002_5</t>
   </si>
   <si>
@@ -237,6 +368,13 @@
     <t>migration_saving_tip.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;
+  &lt;div&gt;ការសន្សំប្រាក់ពិតជាសំខាន់ខ្លាំងណាស់! ប្រាក់សន្សំរួមចំណែកធ្វើអោយការចំណាកស្រុករបស់អ្នកទទួលបានជោគជ័យ។ ការសន្សំប្រាក់ជួយអោយអ្នកសម្រេចគោលបំណង ដូចជាការបង្កើតមុខរបរ ឬរៀនជំនាញជាក់លាក់សម្រាប់ខ្លួនឯងពេលត្រលប់មកស្រុកវិញ ព្រមទំាងជួយស្តារស្ថានភាព ឬជីវភាពគ្រួសារ ប្រើប្រាស់ក្នុងគ្រាអាសន្នណាមួយ និងជួយគាំទ្រការសិក្សាកូនៗ។&lt;/div&gt;
+  &lt;p&gt;ប្រាក់សន្សំ ជាប្រាក់ដែលអ្នកទុកដាច់ដោយឡែកក្រោយពីទូទាត់រាល់ការចំណាយទាំងអស់ ដូចជា ការបង់ថ្លៃផ្ទះ ឬបន្ទប់ជួល ថ្លៃទឹកភ្លើង ការចំណាយលើម្ហូបអាហារប្រចាំថ្ងៃ និងការចំណាយចំាបាច់ផ្សេងៗ ព្រមទំាងប្រាក់ផ្ញើត្រឡប់មកផ្ទះផងដែរ។&lt;/p&gt;
+  &lt;p&gt;អ្នកអាចរៀបចំផែនការសន្សំប្រាក់របស់អ្នកដោយគិតលើទឹកប្រាក់ដែលអ្នកចង់ទទួលបានធៀបនឹងរយៈពេលនៃការសន្សំរបស់អ្នក។ ឧទាហរណ៌ អ្នកចង់បានប្រាក់ ៦០០ដុល្លារក្នុងរយៈពេលពីរឆ្នាំ ដូចនេះអ្នកត្រូវដកទុកចំនួន ២៥ដុល្លារ ក្នុងមួយខែជាប្រចាំ។​ អ្នកអាចទុកដាក់លុយនៅកន្លែងដែលអ្នកគិតថាមានសុវត្ថិភាពបំផុត ដូចជា ប្រអប់សុវត្ថិភាព រឺបើកគណនីសន្សំនៅធនាគារណាមួយ។&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>de_003</t>
   </si>
   <si>
@@ -267,6 +405,36 @@
     <t>coming_home_prepare_plan.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ឥឡូវកុលាបឯងត្រលប់មកស្រុកវិញ ខ្ញុំសូមសួរបទពិសោធកុលាបផ្ទាល់ តើយើងគួរធ្វើអ្វីខ្លះនៅពេលយើងសម្រេចចិត្តត្រលប់មករស់នៅក្នុងសហគមន៍យើងវិញ?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ខ្ញុំបានសង្កេត និងរៀនសូត្រពីអ្នកមុនខ្លះ ខ្ញុំគិតថាសំខាន់ណាស់ដែលយើងត្រូវគិត និងធ្វើផែនការសម្រាប់ក្រោយពេលធ្វើចំណាកស្រុក។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ផែនការយ៉ាងម៉េចទៅ ខ្ញុំហាក់ដូចជាមិនសូវយល់សោះ?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;
+    &lt;div style='flex: 1'&gt;
+      &lt;div&gt;ផែនការ គឺដូចជាអ្វីដែលយើងរៀបចំមុនពេលធ្វើចំណាកស្រុកអញ្ចឹង។ ឥឡូវជាពេលដែលត្រូវគិត តើរៀបចំអ្វីខ្លះសម្រាប់ត្រលប់ និងរស់នៅក្នុងស្រុកវិញ។ ជាដំបូង គឺរៀបចំការធ្វើដំណើរត្រលប់ទៅស្រុកវិញ។ ខ្ញុំបានប្រាប់ឪពុកម្តាយ និងក្រុមគ្រួសារពីថ្ងៃខែ និងពេលវេលានៃការធ្វើដំណើររបស់ខ្ញុំ។ &lt;/div&gt;
+      &lt;p&gt;ហើយខ្ញុំក៏គិតគ្រប់ជ្រុងជ្រោយផងដែរលើការធ្វើដំណើររបស់ខ្ញុំ។ អ៊! ម៉ាលីសឯងមានចាំទេ អំពីការជួញដូរមនុស្សដែលអាចកើតមានគ្រប់ពេល និងទីកន្លែង ដូច្នេះខ្ញុំប្រុងប្រយ័ត្នណាស់ក្នុងការធ្វើដំណើរត្រលប់មកវិញ គឺខ្ញុំមិនធ្វើដំណើរជាមួយអ្នកមិនស្គាល់មុខទេ ហើយខ្ញុំធ្វើដំណើរត្រលប់ជាក្រុមជាមួយបងប្អូន សាច់ញាត្តិដែលខ្ញុំទុកចិត្តបំផុត។&lt;/p&gt;
+      &lt;p&gt;រឿងសំខាន់មួយទៀតនោះគឺ ខ្ញុំបានគិតពីមុខរបរ និងការងារអ្វីដែលខ្ញុំចង់ធ្វើ ឬអាចធ្វើបាន។ តើជំនាញអ្វីខ្លះដែលត្រូវការនៅក្នុងសហគមន៍ ឬតំបន់នៅក្បែរស្រុកភូមិរបស់យើង។ &lt;/p&gt;
+      &lt;p&gt;បន្ថែមទៀត ខ្ញុំគិត តើខ្ញុំនឹងត្រៀមខ្លួនចូលទៅរស់នៅជាមួយនឹងក្រុមគ្រួសារ និងសហគមន៍យ៉ាងម៉េចដែរ? ព្រោះខ្ញុំបានរស់នៅ និងធ្វើការនៅប្រទេសថៃយូរដែរ។ ខ្ញុំបានគិតថា តើខ្ញុំធ្វើដូចម្តេច ប្រសិនមានការរើសអើងពីសមាជិកគ្រួសារខ្លះ ឬអ្នកភូមិខ្លះនៅក្នុងសហគមន៍?&lt;/p&gt;
+      &lt;p&gt;តើខ្ញុំអាចភ្ជាប់ខ្លួនយើងទៅនឹងបណ្តាញគំាទ្រដែលមាននៅក្នុងសហគមន៍យ៉ាងម៉េច?ដើម្បីទទួលបានព័ត៌មានអំពីការងារ និងការគាំពារផ្នែកសង្គមផ្សេងៗ រួមទាំងសេវាអំពើហិង្សាលើស្រ្តីផងដែរ។&lt;/p&gt;
+      &lt;p&gt;លើសពីនេះទៀត ខ្ញុំក៏បានចែករំលែកបទពិសោធនៃការទៅធ្វើការនៅប្រទេសថៃជាមួយបងប្អូន និងអ្នកភូមិផ្សេងទៀតដែរ។ ព័ត៌មានពិត ត្រឹមត្រូវពីចំណាកស្រុក គឺជួយឲ្យយើងមានការរៀបចំសម្រាប់ការធ្វើចំណាកស្រុក។&lt;/p&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ចុះអារម្មណ៍វិញយ៉ាងម៉េចដែរ?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ពេលខ្លះខ្ញុំក៏នឹកពេលវេលា ការចងចាំល្អៗមួយចំនួនផងដែរ។ ជាពិសេសមិត្តរួមការងារជិតស្និតពីរបីនាក់ តែខ្ញុំមិនសោកស្តាយចំពោះការសម្រេចចិត្តរបស់ខ្ញុំទេ។&lt;/div&gt;
+  &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>de_003_2</t>
   </si>
   <si>
@@ -279,6 +447,9 @@
     <t>coming_home_back_home.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;ការត្រលប់មករស់នៅជាមួយគ្រួសារវិញមានទាំងអារម្មណ៍រំភើប និងការបន្សាំខ្លួនចូលទៅក្នុងរបៀបរស់នៅរបស់គ្រួសារអ្នកវិញ។ ជាការចាំបាច់ដែលអ្នកនិយាយប្រាប់ទៅគ្រួសារ រួមមានឳពុកម្តាយ បងប្អូនស្រី ឬមិត្តភក្តិជិតស្និទ្ធរបស់អ្នកពីអារម្មណ៍របស់អ្នក អ្វីដែលអ្នកចង់ធ្វើ និងពីរបៀបរស់នៅប្រចាំថ្ងៃបែបថ្មីរបស់អ្នក។&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>de_003_3</t>
   </si>
   <si>
@@ -321,6 +492,52 @@
     <t>violence_on_women.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;
+  &lt;ul&gt;
+    &lt;li&gt;អំពីហិង្សាលើស្ត្រី គឺជាទង្វើអំពើហិង្សាដែលទាក់ទងនឹងយេនឌ័រដែលនាំឲ្យមាន ឬទំនងជាបង្កអោយមានគ្រោះថ្នាក់ ឬការឈឺចាប់ផ្លូវកាយ ផ្លូវភេទ ឬផ្លូវចិត្តដល់ស្រ្តីរួមនឹងការគំរាមកំហែងប្រព្រឹត្តទង្វើទំាងនេះ ការបង្ខិតបង្ខំ ការបំបិទសេរីភាពតាមអំពើចិត្តមិនថាកើតមានឡើងនៅទីសាធារណៈ ឬ ជីវិតឯកជននោះទេ។&lt;/li&gt;
+    &lt;li&gt;អំពីហិង្សាលើស្ត្រីគ្រប់ទម្រង់ គឺជាការរំលោភសិទ្ធិស្រ្តី។&lt;/li&gt;
+  &lt;/ul&gt;
+  &lt;h2&gt;ទម្រង់ផ្សេងៗអំពើហិង្សាលើស្រ្តី&lt;/h2&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 130px;'&gt;ហិង្សាផ្លូវកាយ៖&lt;/div&gt;&lt;div style='flex: 1'&gt;វាយដំ ឬដាល់ រុញឲ្យដួល ទះ តប់ គប់ដោយប្រើរបស់ផ្សេងៗ ការខំា ការទាញសក់ ការកាត់ ឬចាក់ ការធ្វើអោយថប់ដង្ហើម និងការដុត ។ល។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 130px;'&gt;ហិង្សាផ្លូវចិត្ត៖&lt;/div&gt;
+    &lt;div style='flex: 1'&gt;
+      &lt;ul style='marginTop: 0;'&gt;
+        &lt;li&gt;ជេរប្រមាថ មើលងាយ ឬសម្លុតគំរាមកំហែង&lt;/li&gt;
+        &lt;li&gt;មិនគោរព ផ្តល់តម្លៃ និងទំនុកចិត្ត&lt;/li&gt;
+        &lt;li&gt;និយាយចំអកបញ្ឈឺចិត្ត និងធ្វើអោយអាម៉ាសមុខ&lt;/li&gt;
+        &lt;li&gt;ការបដិសេដលើគំនិត និងយោបល់&lt;/li&gt;
+        &lt;li&gt;គ្រប់គ្រង និងបំបិតសិទ្ធសេរីភាព&lt;/li&gt;
+        &lt;li&gt;បដិសេធមិនគោរពនូវជំនឿ&lt;/li&gt;
+        &lt;li&gt;ការរំពឹងចង់បានច្រើនហួសហេតុ&lt;/li&gt;
+        &lt;li&gt;ចេះតែរិះគន់ឥតឈប់ឈរ&lt;/li&gt;
+        &lt;li&gt;ទាមទារអ្វីៗដោយមិនសមហេតុផល&lt;/li&gt;
+        &lt;li&gt;និយាយចោទប្រកាន់ ស្តីបន្ទោស គំរាម ឬបង្គាប់បញ្ជា&lt;/li&gt;
+      &lt;/ul&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 130px;'&gt;ហិង្សាផ្លូវភេទ៖&lt;/div&gt;
+    &lt;div style='flex: 1'&gt;ការរំលោភសេពសន្ថវៈ, ការរំលោភសេពសន្ថវៈក្នុងចំណងអាពាហ៍ពិពាហ៍, ស្មន្ធការ (ការរួមភេទជាមួយសាច់ញាតិខ្លួនឯង), បៀតបៀនផ្លូវភេទ, រុកគួនខាងផ្លូវភេទ, បង្ហាញកេរភេទ, ការនិយាយទាក់ទងផ្លូវភេទដែលមិនសមរម្យ ឬសំដែងឥរិយាបទផ្លូវភេទដែលធ្វើឲ្យមានការភ័យខ្លាច, ការប៉ះពាល់រាងកាយ ឬកេរិ៍្តភេទដោយចេតនា, ការបង្ខំឲ្យធ្វើសកម្មភាពផ្លូវភេទ ដូចជាបង្ខំឲ្យរួមភេទតាមមាត់, មើលរឿងអាសអាភាស, ផលិតសម្ភារៈ ឬឧបករណ៍អាសអាភាស ឬមើលសកម្មភាពរួមភេទ ឬលើកទឹកចិត្តអោយប្រព្រឹត្តអាកប្បកិរិយាទាក់ទងនឹងផ្លូវភេទមិនសមរម្យ។ល។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 130px;'&gt;ហិង្សាផ្នែកសេដ្ឋកិច្ច៖&lt;/div&gt;
+    &lt;div style='flex: 1'&gt;មិនអនុញ្ញាតឱ្យទទួលបានអាហារ ប្រាក់កាស សម្លៀកបំពាក់ ថ្នាំសង្កូវ ការអប់រំ មិនអនុញ្ញាតឱ្យទៅធ្វើការងារ បង្ខំឱ្យធ្វើការងារ ដកហូតប្រាក់ចំនូលទាំងអស់ ពុំផ្តល់សិទ្ធិកាន់កាប់ទ្រព្យសម្បត្តិ&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ខ្ញុំបានឮថាបងប្អូនស្រ្តីពលករចំណាកស្រុកជួបនូវបទពិសោធអំពើហិង្សា តើកុលាបមានដែលឭ ឬឃើញអំពីហិង្សាលើស្រ្តីទេ?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ខ្ញុំបានដឹងរឿងមិត្តរួមការងារជិតស្និតម្នាក់ គឺរស្មី។ រស្មីគាត់រៀបការប្រមាណជាង៣ឆ្នាំហើយ ​ជាមួយនឹងប្តី របស់គាត់ឈ្មោះវិច្ឆិកា ដែលធ្វើការនៅថៃទាំងពីរនាក់។ រស្មីប្រាប់ខ្ញុំថា មុនរៀបការ វិច្ឆិកា គឺប្រចណ្ទ័ខ្លាំងណាស់។ តែពេលណុង៎ រស្មីគិតថាដោយសារតែគាត់ស្រលាញ់នាងខ្លាំងពេក។ ដល់ពេលរៀបការហើយ ប្តីរបស់រស្មី គឺមិនចង់ឲ្យគាត់រាប់អានមិត្តភក្តិ ឬធ្វើការកន្លែងបែកពីគ្នាទេ។ ប៉ុន្តែប្តីរបស់រស្មីវិញ ឲ្យតែបើកប្រាក់ខែម្តងៗ ដឹងតែដើរលេងជាមួយនិងគូរកនរបស់គេដាច់យប់រហូត។ រស្មីបានប្រាប់ខ្ញុំទៀតថា ពេលមួយនោះ ក្រោយពីបើកប្រាក់ខែហើយ ប្តីគេដើរសប្បាយដល់យប់ជ្រៅ ស្រាប់តែមកដល់ផ្ទះរករឿង ថារស្មីមានប្រុសអីណា​ ដោយគ្មានហេតុផលអីសោះ ដល់ពេលនាងប្រកែក ប្តីនាងបានទះកំផ្លៀង និងរុញឲ្យដួល។​ ក្រោយមក វិច្ឆិកាបានមកសុំទោសដែលបានជ្រុលដៃទះកំផ្លៀងប្រពន្ធ និងសន្យាមិនធ្វើអញ្ចឹងទៀតទេ។ មិនបានប្រហែលមួយអាទិត្យផង ប្តីរស្មីបានធ្វើទង្វើនេះដដែល ហើយកាន់តែអាក្រក់ជាងមុនទៅទៀត គឺបានដាល់មុខរស្មីមួយដៃយ៉ាងធ្ងន់។ &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ដល់ថ្នាក់ហ្នឹងផង! វិច្ឆកានោះពិតជាអាក្រក់មែន គេគួរតែត្រូវបានទទួលទោសចំពោះទង្វើហិង្សាដែលគេបានប្រព្រឹត្តិមកលើរស្មី។ តែជាការល្អណាស់ ដែលរស្មីមានមិត្តល្អដូចកុលាបឯង ព្រោះនាងមាន មិត្តល្អដែលអាចទុកចិត្តនិយាយរឿងរ៉ាវក្នុងចិត្តប្រាប់បាន។&lt;/div&gt;
+  &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>sa_001_2</t>
   </si>
   <si>
@@ -333,6 +550,30 @@
     <t>harassment.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;
+  &lt;div&gt;ការបៀតបៀនផ្លូវភេទ គឺជាទង្វើ ឬឥរិយាបថទាំងឡាយណាដែលមិនចង់បាន មិនស្វាគមន៍ ឬក៏មិនអនុញ្ញាតពាក់ព័ន្ធនឹងផ្លូវភេទដែលធ្វើអោយបុគ្គលម្នាក់ ឬច្រើននាក់មានអារម្មណ៍អាម៉ាស់មុខ ភិតភ័យ ឬអាក់អន់ចិត្ដ។ ការបៀតបៀនផ្លូវភេទមានទម្រង់ខុសគ្នារួមមាន៖ ការបៀតបៀនផ្លូវភេទដោយប្រើអំណាច ពាក្យសម្ដី សំលេង និងការបៀតបៀនផ្លូវភេទដោយកាយវិការ ។&lt;/div&gt;
+  &lt;div style='color: red; margin-top: 10px'&gt;ឧទាហរណ៍ ការបៀតបៀនផ្លូវភេទដោយពាក្យសម្ដី&lt;/div&gt;
+  &lt;ul&gt;
+    &lt;li&gt;ការប្រើប្រាស់ភាសាមិនសមរម្យ ឬភាសាអាសអាភាស និងនិយាយលេងសើចបែបអាសអាភាស&lt;/li&gt;
+    &lt;li&gt;ការហៅមិនសមរម្យទៅកាន់ស្រ្ដីនៅតាមផ្លូវ ឬការប្រើភាសាអាសអាភាសនៅពេលស្រ្តីដើរកាត់&lt;/li&gt;
+    &lt;li&gt;ការហូចបែបមិនសមរម្យនៅពេលស្រ្តីដើរកាត់&lt;/li&gt;
+    &lt;li&gt;សំណើរ និងការលួងលោមដដែលៗ ដើម្បីបំពេញចំណង់ផ្លូវភេទ ឬការណាត់ជួបក្នុងគោលបំណងផ្លូវភេទ&lt;/li&gt;
+    &lt;li&gt;ការនិយាយសម្តីដែលមានលក្ខណៈផ្លូវភេទ (ឧទាហរណ៍៖ ហៅឈ្មោះជាលក្ខណៈផ្លូវភេទ ឬសួរអំពីអត្តសញ្ញាណផ្លូវភេទ ឬការប្រព្រឹត្តខាងផ្លូវភេទ)&lt;/li&gt;
+    &lt;li&gt;ការវាយប្រហារឯកជនភាព ទាំងក្នុង និងក្រៅសាលារៀន ឬកន្លែងធ្វើការ (ឧទាហរណ៍៖ការបៀតបៀន ដោយការហៅទៅទូរស័ព្ទ ឬដើរតាមស្រ្ដីនោះដល់ផ្ទះ)&lt;/li&gt;
+    &lt;li&gt;ការស្នើដាក់លក្ខខណ្ឌដោះដូរដើម្បីបំពេញចំណង់ផ្លូវភេទផ្ទាល់ខ្លួន ដូចជា ការផ្ទេរ ការដំឡើងឋានៈ ប្រាក់ខែ ឬបន្ដការងារ&lt;/li&gt;
+    &lt;li&gt;គំរាមកំហែងវាយធ្វើបាប បង្ខិតបង្ខំ ឬរំលោភផ្លូវភេទ។&lt;/li&gt;
+  &lt;/ul&gt;
+  &lt;div style='color: red;'&gt;ឧទាហរណ៍ ការបៀតបៀនផ្លូវភេទដោយកាយវិការ&lt;/div&gt;
+  &lt;ul&gt;
+    &lt;li&gt;ការតាំងបង្ហាញវត្ថុដែលធ្វើឱ្យនឹកឃើញដល់ផ្លូវភេទ ដូចជារូបភាព ទស្សនាវដ្ដី ផ្ទាំងរូបភាព ឬតុក្កតាអាសអាភាស&lt;/li&gt;
+    &lt;li&gt;ការសម្លក់សម្លឹង ឬសញ្ញាកាយវិការដែលទាក់ទងនឹងផ្លូវភេទ&lt;/li&gt;
+    &lt;li&gt;ការប៉ះ ការថើប ការឱបក្រសោប ការធ្វើសរសៃ ឬការអង្អែលលើរាងកាយដែលមិនអនុញាត&lt;/li&gt;
+    &lt;li&gt;ការវាយធ្វើបាប ឬបង្ខិតបង្ខំ និងរំលោភផ្លូវភេទ &lt;/li&gt;
+  &lt;/ul&gt;
+  &lt;div&gt;ទោះបីជានរណាក៏អាចជាកម្មវត្ថុនៃអំពើបៀតបៀនផ្លូវភេទ ស្រ្តីភាគច្រើនត្រូវបានក្លាយជាជនរងគ្រោះនៃការបៀតបៀនផ្លូវភេទ។ ទម្រង់នៃការការបៀតបៀនផ្លូវភេទ គឺអាចកើតមាននៅគ្រប់ទីកន្លែងទាំងអស់ រួមទាំងកន្លែងធ្វើការ។ នៅកន្លែងធ្វើការ ការបៀតបៀនផ្លូវភេទពេលខ្លះ គឺជាទង្វើមួយដែលជម្រុញឲ្យទទួលយកជាថ្នូរ និងផលប្រយោជន៍ត្រលប់មកវិញ។ ជាក់ស្តែង ការស្នើដាក់លក្ខខណ្ឌដោះដូរដើម្បីបំពេញចំណង់ផ្លូវភេទផ្ទាល់ខ្លួន ដូចជា ការផ្ទេរ ការដំឡើងឋានៈ ប្រាក់ខែ ឬបន្ដការងារ។&lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>sa_001_3</t>
   </si>
   <si>
@@ -345,6 +586,20 @@
     <t>your_health.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;
+  &lt;div&gt;ការថែទាំសុខភាពរបស់អ្នក គឺមានសារៈសំខាន់ណាស់ ទន្ទឹមនឹងពេលដែលអ្នកខ្វល់ខ្វាយ និងរវល់ជាមួយការងារប្រចាំថ្ងៃ។ &lt;/div&gt;
+  &lt;ul&gt;
+    &lt;li&gt;មិនមែនជាការខ្មាស់អៀននោះទេក្នុងការនិយាយអំពីបទពិសោធ ឬចំងល់ផ្សេងៗទាក់ទងនឹងការមករដូវរបស់អ្នក។ មិត្តភក្តិជិតស្និទ្ធ ឬបងប្អូនស្រី ឬម្តាយអាចជាមនុស្សដែលគួរឲ្យទុកចិត្ត និងមានអារម្មណ៍សុវត្ថិភាពសម្រាប់អ្នកក្នុងការនិយាយប្រាប់អំពីកង្វល់ ឬការព្រួយបារម្ភផ្សេងៗអំពីការមករដូវរបស់អ្នក។&lt;/li&gt;
+    &lt;li&gt;ជាធម្មតា ស្រ្តីមករដូវជារៀងរាល់ចន្លោះពី ២៨ ទៅ ៤០ ថ្ងៃ ដែលជាវដ្តទូទៅ ហើយជារឿងធម្មតា។ រដូវ ទៀង គឺមានន័យថាមកជារៀងរាល់ ២៨ ថ្ងៃម្តង។ ប៉ុន្តែជាករណីកម្រដែលស្រ្តីមករដូវទៀងក្នុងកំឡុងពេល ២៨ថ្ងៃ។ ស្រ្តីខ្លះអាចមករដូវក្នុងកំឡុងពេល ៣០ ថ្ងៃ អ្នកខ្លះ ៣១ ថ្ងៃ ឬអ្នកខ្លះ ៣៥ ថ្ងៃ លើសពីនេះទៀតមានអ្នកខ្លះរហូតដល់ ៤០ ថ្ងៃ។&lt;/li&gt;
+    &lt;li&gt;យុវតី និងស្រ្តីមានការព្រួយបារម្ភពីការធ្លាក់សរបស់ពួកគេ។ ជាធម្មតា ស្រ្តីមានការធ្លាក់សមុនមករដូវ និងក្រោយមករដូវ។ នេះជារឿងធម្មតាទេ។ ប៉ុន្តែ ប្រសិនបើការធ្លាក់ស របស់អ្នកមានធុំក្លិន មានពណ៌ដូចជាសំបោរពណ៌លឿង អ្នកគួរតែរកការពិគ្រោះយោបល់ជាមួយគ្រូពេទ្យខាងផ្នែករោគស្រ្តី។ &lt;/li&gt;
+    &lt;li&gt;អនាម័យនៅពេលមានរដូវ ដូចជាការលាងសម្អាតឲ្យបានញឹកញាប់ ការប្តូរសំឡីអនាម័យ ឬក្រណាត់ទ្រាប់ ជារៀងរាល់ ៣ ទៅ ៤ ម៉ោង ការហូបអាហារមានបន្លែ ផ្លែឈើ និងហូបទឹកឲ្យបានច្រើន សម្រាកឲ្យបានគ្រប់គ្រាន់ គឺជួយនាំមកនូវសុខភាពបន្តពូជល្អ និងរឹងមាំ។&lt;/li&gt;
+    &lt;li&gt;ការស្វែងរកការពិគ្រោះយោបល់ជាមួយគ្រូពេទ្យខាងផ្នែករោគស្រ្តី គឺមានសារៈសំខាន់ណាស់។ កុំភ្លេចណា៎ ការនិយាយពីការមករដូវ ឬសុខភាពបន្តពូជ មិនមែនជារឿងខ្មាស់អៀនទេ!!!&lt;/li&gt;
+    &lt;li&gt;អ្នក គឺជាម្ចាស់លើរាងកាយរបស់អ្នក។ អ្នកមានសិទ្ធិធ្វើសេចក្តីសម្រេចចិត្តលើផែនការពន្យារកំណើត និងការកំណត់ចំនួនកូនដែលអ្នកចង់បាន។ មានជម្រើសជាច្រើន ដូចជា ការប្រើប្រាស់ស្រោមអនាម័យ ថ្នាំចាក់ ថ្នាំគ្រាប់ កងដាក់ក្រោមស្បែក និងកងដាក់ក្នុងស្បូន ដែលជាសេវាសុខភាពសាធារណៈ ហើយអាចរកសេវានេះបាន ដូចជា មណ្ឌលសុខភាព ឬមន្ទីរពេទ្យបង្អែកជាដើម ដែលជាមធ្យោបាយមានប្រសិទ្ធិភាពខ្ពស់សម្រាប់ការពន្យាកំណើត។ មធ្យោបាយពន្យាកំណើតបែបធម្មជាតិ ដូចជាតាមរយៈការបំបៅដោះកូន តាមរយៈប្រតិទិន តាមរយៈការដកទឹកកាមចេញ។ ប្រសិទ្ធភាពរបស់វា គឺមិនមានខ្ពស់ទេ ហើយប្រឈមនឹងមានផ្ទៃពោះដោយមិនចង់បាន ឬចៃដន្យ។ &lt;/li&gt;
+  &lt;/ul&gt;
+  &lt;div&gt;កុំភ្លេច ពិគ្រោះយោបល់ជាមួយគ្រូពេទ្យជំនាញ នៅពេលអ្នកចង់ធ្វើផែនការពន្យាកំណើត។ ស្វែងយល់ពីផលប៉ះពាល់ និងប្រសិទ្ធិភាពនៃមធ្យោបាយពន្យារកំណើតនិមួយៗ ជាការចាំបាច់!&lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>sa_001_4</t>
   </si>
   <si>
@@ -357,6 +612,38 @@
     <t>understand_exploitation_and_human_traficking.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ខ្ញុំបានឮអ្នកភូមិ មេក្រុម មេភូមិ និយាយអីទេថាបងប្អូនស្រ្តីពលករចំណាកស្រុកប្រយត្ន័ត្រូវគេជូញដូរ។ តើយ៉ាងម៉េចវិញ កុលាប? ក្រែងយើងទៅធ្វើការ ចុះហេតុអី្វបានជា គេអាចជួញដូរ ឬកេងប្រវញ្ច័យើងបានយ៉ាងម៉េចវិញ?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px'&gt;កុលាប៖&lt;/div&gt;
+    &lt;div style='flex: 1'&gt;
+      ខ្ញុំធ្លាប់បានចូលរួមវគ្គបណ្តុះបណ្តាលទាក់ទងអំពីជួញដូរមនុស្ស និងការកេងប្រវញ្ច័ ខ្ញុំអាចប្រាប់ម៉ាលីសបានណា។
+      &lt;p&gt;ការជួញដូរមនុស្ស គឺជាការជ្រើសរើស ការដឹកជញ្ជូន ការផ្ទេរ ការឃាត់ទុក ឬការផ្តល់ទីជម្រក តាមមធ្យោបាយគំរាមគំហែង ការប្រើកម្លាំង ទម្រង់ផ្សេងទៀតនៃការបង្ខិតបង្ខំ ការចាប់ ពង្រត់ ការក្លែងបន្លំឯកសារ ការបោកប្រាស់ ការរំលោភបំពានអំណាច ការប្រើតួនាទីរំលោភជនរងគ្រោះ ការឲ្យ ឬទទួលយកកម្រៃ ឬអត្ថប្រយោជន៍ណាមួយដើម្បីសម្រេចបានការព្រមព្រៀងឲ្យមានការត្រួតត្រាលើមនុស្សម្នាក់ទៀត។ ការកេងប្រវ័ញ្ចរួមមាន ការកេងប្រវ័ញ្ចលើពេស្យាកម្មជនដទៃ ឬទម្រង់ផ្សេងៗទៀតនៃការកេងប្រវ័ញ្ចផ្លូវភេទ ពលកម្ម ឬសេវាដោយបង្ខំ ទាសភាព ឬការអនុវត្តន៍ស្រដៀងគ្នានឹង ទាសភាព ទាសករ ឬការដកហូតសរីរាង្គណាមួយ។&lt;/p&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ស្តាប់ទៅ ខ្ញុំដូចជានៅមិនទាន់យល់បានច្បាស់ តើកុលាបអាច ឧទាហរណ៍អ្វីបន្ថែមទៀតមើល។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ខ្ញុំមានរឿងមួយដែលខ្ញុំបានដឹងពីអ្នកធ្វើការជាមួយគ្នា កាលនៅប្រទេសថៃ។ មានស្ត្រីម្នាក់ឈ្មោះចិន្តា គាត់បានដឹងតាមរយៈបុរសម្នាក់នៅក្នុងភូមិ ថានៅប្រទេសថៃមានឳកាសច្រើននឹងអាចរកការងារធ្វើបាន ។ បុរសនោះជាមេខ្យល់នំាមនុស្សទៅធ្វើការនៅរោងចក្រនៅប្រទេសថៃ។ ហើយបានប្រាប់ចិន្តាថា ការចំណាកស្រុកអស់លុយតិចតួចទេ ព្រមទំាងមិនចាំបាច់ចំណេយលើថ្លៃធ្វើឯកសារ ក៏អាចទៅធ្វើការបានដូចគ្នា។ បុរសនោះប្រាប់ចិន្តា កុំឲ្យមានការបារម្ភអ្វីទាំងអស់ គាត់ធានាថាគ្រប់យ៉ាងនឹងគ្មានបញ្ហា ចិន្តានឹងបានការងារធ្វើនៅប្រទេសថៃ ហើយមានប្រាក់ខែខ្ពស់។ លឺសំដីបុរសនោះ ធានាបែបនេះ ចិន្ថាក៏ជឿជាក់។ បុរសនោះតម្រូវឲ្យចិន្តា បង់លុយមួយចំនួន ដើម្បីធ្វើដំណើរទៅធ្វើការទៅប្រទេសថៃ។ ម៉ាលីសដឹងអត់ ថាចិន្តាធ្វើដំណើរបែបណាដើម្បីចូលទៅប្រទេសថៃ?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ប្រាប់មកកុលាប ថាចិន្ថាទៅដោយរបៀបណា? &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ចិន្តាត្រូវលាក់ខ្លួននៅក្នុងឡានដឹកទំនិញដើម្បីឆ្លងដែន។ ពេលគាត់ទៅដល់ស្រាប់តែគេប្រាប់ថា រោងចក្រមិនទាន់បើកឲ្យដំណើរការនោះទេ។ ប៉ុន្តែចិន្តាអាចធ្វើការនៅបារមួយកន្លែងនៅទីក្រុងដ៏ធំនោះ។ ម្ចាស់បារបានផ្តល់កន្លែងស្នាក់នៅឲ្យចិន្តា និងបានដកលិខិតឆ្លងដែនរបស់នាងទុក។ ហើយក៏មិនឲ្យចិន្តាប្រើប្រាស់ទូរស័ព្ទបានដែរ។ 2-3ថ្ងៃក្រោយមក ចិន្ថាក៏បានដឹងថា នារីទាំងអស់នៅទីនោះ គឺត្រូវរួមភេទជាភ្ញៀវដើម្បីបានលុយ ហើយនាងត្រូវបានគេបង្ខំឲ្យធ្វើបែបនោះដូចគ្នាដែរ។ ចិន្តាបានព្យាយាម រត់ចេញពីទីនោះ ប៉ុន្តែនាងត្រូវបានគេ បង្ខាំមិនឲ្យចេញទៅណាបានទេ ហើយម្ចាស់បារនោះ បានប្រាប់ចិន្តាថា នាងបានជំពាក់លុយគេច្រើនណាស់ លើការចំណាយឲ្យនាងបានមកដល់ទីនេះ អញ្ចឹងហើយ នាងត្រូវតែធ្វើការដើម្បីដោះបំណុលទាំងអស់នោះ។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ពិតជាអាក្រក់មែន បោកបញ្ឆោត ភូតកុហក បង្ខំឲ្យចិន្តាធ្វើការដែលនាងមិនចង់ធ្វើ ហើយថានាងជាកូនបំណុលទៀតទាំងដែលចិន្តាមិនធ្លាប់បានខ្ចីលុយថៅកែនោះផង។ ចំណែកឯ បុរសដែលសន្យារកការងារឲ្យចិន្តាធ្វើ និងថាបានប្រាក់ខែច្រើននោះវិញ ពិតជាសំបូរល្បិចគេចកល បោកបញ្ចោត ដើម្បីឲ្យចិន្តាមានការជឿជាក់ បានជាចិន្តាត្រូវបានធ្លាក់ចូលអន្ទាក់នៃការកេងប្រវញ្ច័ផ្លូវភេទបែបនេះ។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ស្តាប់ហើយខឹងយ៉ាងនេះ ប្រហែលជាម៉ាលីសឯងយល់ច្បាស់ហើយមើលទៅ!&lt;/div&gt;
+  &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>sa_001_5</t>
   </si>
   <si>
@@ -387,6 +674,19 @@
     <t>urgent_leave.png</t>
   </si>
   <si>
+    <t>&lt;div&gt;
+  &lt;div&gt;តើអ្នកនឹងត្រូវការអ្វីខ្លះ ប្រសិនជាអ្នកតម្រូវឱ្យចាកចេញបន្ទាន់?&lt;/div&gt;
+  &lt;ul&gt;
+    &lt;li&gt;ប្រសិនបើអ្នកត្រូវ ឬសម្រេចចិត្តចាកចេញក្នុងស្ថានភាពបន្ទាន់ វាជារឿងសំខាន់ណាស់ដែលអ្នកត្រូវគិតគូរពីលុយកាក់ ទ្រព្យធន ឯកសារសំខាន់ និងសំភារៈមួយចំនួនដែលអ្នកនឹងត្រូវការ។&lt;/li&gt;
+    &lt;li&gt;ការសន្សំលុយ និងលាក់វានៅកន្លែងណាមួយដែលអ្នកអាចយកបានយ៉ាងលឿន និងងាយស្រួល ប្រសិនបើអ្នកត្រូវចាកចេញដោយប្រញាប់។ វាអាចជាលុយ កាតអេធីអ៊ីម (កាតសម្រាប់ដកលុយដោយស្វ័យប្រវត្តិ) ដែលអ្នកត្រូវមានសម្រាប់ចំណាយលើថ្លៃធ្វើដំណើរ និងចំណាយផ្សេងៗ។ គិតដល់មិត្ត ឬអ្នកជិតខាងដែលអាចជួយបញ្ជូលលុយ ទូរស័ព្ទអោយអ្នកនៅពេលត្រូវការប្រើបន្ទាន់។&lt;/li&gt;
+    &lt;li&gt;រក្សាទុកអត្តសញ្ញាណប័ណ្ណ ឬលិខិតឆ្លងដែនរបស់អ្នក និងកូននៅកន្លែងដែលលាក់បាំងដែលអាចយកបានភ្លាមៗ។&lt;/li&gt;
+    &lt;li&gt;ស្តុកទុកនូវរបស់ដែលអ្នកត្រូវការដូចជា អាហារ សំល្លៀកបំពាក់ជាដើម ដែលអ្នកងាយស្រួលយកបាន។&lt;/li&gt;
+    &lt;li&gt;វេចខ្ចប់កាតាបសង្គ្រោះបន្ទាន់សម្រាប់ខ្លួនអ្នក និងលាក់វានៅកន្លែងមានសុវត្ថិភាពនៅផ្ទះអ្នកជិតខាង ឬមិត្តភក្តិដែលអាចជឿទុកចិត្តបាន។&lt;/li&gt;
+    &lt;li&gt;បិទការតាមដានទីតាំងក្នុងទូរស័ព្ទ និងឧបករណ៌អេឡិចត្រូនិចផ្សេងៗរបស់អ្នកដែលមានមុខងារស្វែងរកទីតាំងរបស់អ្នក បើសិនជាអ្នកគិតថាត្រូវចាកចេញ។ ត្រូវចង់ចាំថាវាអាចឱ្យអ្នកប្រព្រឹត្តអំពើរំលោភបំពានលើអ្នកតាមដានអ្នកតាមប្រព័ន្ធអនឡាញបាន។&lt;/li&gt;
+  &lt;/ul&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>sa_002_2</t>
   </si>
   <si>
@@ -396,6 +696,23 @@
     <t>checklist.png</t>
   </si>
   <si>
+    <t>&lt;div&gt;
+  &lt;div&gt;របស់ដែលត្រូវវេចខ្ចប់ក្នុងកាតាបសង្គ្រោះបន្ទាន់របស់អ្នក&lt;/div&gt;
+  &lt;ul&gt;
+    &lt;li&gt;អត្តសញ្ញាណប័ណ្ណ រួមទាំងរូបថតមួយចំនួន&lt;/li&gt;
+    &lt;li&gt;លិខិតឆ្លងដែន លិខិតអនុញ្ញាតការងារ ទិដ្ឋាការ&lt;/li&gt;
+    &lt;li&gt;ធានារ៉ាប់រង និងឯកសារសំខាន់ៗផ្សេងៗទៀត។&lt;/li&gt;
+    &lt;li&gt;សោរសាគួរសម្រាប់ផ្ទះ ឡាន និងកន្លែងធ្វើការរបស់អ្នក&lt;/li&gt;
+    &lt;li&gt;លុយ កាតអេធីអ៊ីម (កាតសម្រាប់ដកលុយដោយស្វ័យប្រវត្តិ)&lt;/li&gt;
+    &lt;li&gt;សំល្លៀកបំពាក់បន្ថែម និងខោអាវក្នុង&lt;/li&gt;
+    &lt;li&gt;សំឡីអនាម័យ ឬខោទឹកនោមសម្រាប់កូនៗ&lt;/li&gt;
+    &lt;li&gt;ខ្សែសាកទូរស័ព្ទ ហើយបើអាច កាតបញ្ចូលទូរស័ព្ទដែលអាចប្រើបានក្នុងពេលមានអាសន្ន&lt;/li&gt;
+    &lt;li&gt;ថ្នាំមួយចំនួនដែលអ្នក និងកូនអ្នកប្រើជាប្រចាំ&lt;/li&gt;
+    &lt;li&gt;លេខទូរស័ព្ទសំខាន់ៗ&lt;/li&gt;
+  &lt;/ul&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>sa_002_3</t>
   </si>
   <si>
@@ -405,6 +722,18 @@
     <t>thing_need_to_know.png</t>
   </si>
   <si>
+    <t>&lt;div&gt;
+  &lt;div&gt;អ្វីដែលអ្នកត្រូវដឹងបើអ្នកជាស្រ្តីពលករចំណាកស្រុក&lt;/div&gt;
+  &lt;ul&gt;
+    &lt;li&gt;អ្នកមានសិទ្ធទទួលបានសុវត្ថិភាព និងការពារ ទោះបីជាអ្នកមិនមែនជាប្រជាពលរដ្ឋនៅក្នុងប្រទេសអ្នកកំពុងរស់នៅ ឬកំពុងធ្វើការក៏ដោយ។&lt;/li&gt;
+    &lt;li&gt;ទាក់ទងក្រុមស្ត្រី ឬអង្គការស្ត្រី ទូរស័ព្ទទាន់ហេតុការណ៌ មន្រ្តីប៉ូលីស ស្ថានទូត សហជីពពាណិជ្ជកម្ម មជ្ឍមណ្ឌលពលករចំណាកស្រុក គ្លីនិកសុខភាព ឬសេវាផ្សេងៗដែលអ្នកត្រូវការ។&lt;/li&gt;
+    &lt;li&gt;ស្នើសុំសេវាបកប្រែពេលអ្នកស្វែងរកសេវាទូរស័ព្ទជំនួយ ប៉ូលីស មន្ទីរពេទ្យ ឬសេវាផ្សេងៗទៀត។&lt;/li&gt;
+    &lt;li&gt;ភ្ជាប់ទំនាក់ទំនងជាមួយបណ្តាញជួយមិត្ត (ក្រុមស្ត្រី ឬអង្គការស្ត្រី) ដែលអាចផ្តល់ពត៌មាននិងភ្ជាប់អ្នកទៅរកសេវាផ្សេងៗ។&lt;/li&gt;
+    &lt;li&gt;រក្សាទុកលេខទូរស័ព្ទស្ថានទូត និងកុងស៊ុល ពួកគេនៅទីនោះដើម្បីជួយអ្នកនៅក្រៅប្រទេស។&lt;/li&gt;
+  &lt;/ul&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>sa_002_4</t>
   </si>
   <si>
@@ -412,6 +741,16 @@
   </si>
   <si>
     <t>safety_more_strategy.png</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;
+  &lt;div&gt;យុទ្ធសាស្រ្តដើម្បីសុវត្ថិភាពផ្សេងទៀត&lt;/div&gt;
+  &lt;ul&gt;
+    &lt;li&gt;មានពាក្យសម្ងាត់ ឬសញ្ញាសម្គាល់ ឬឃ្លាសុវត្ថិភាពសំរាប់ប្រើជាមួយមិត្តភក្តិ ឬក្រុមគ្រួសាររបស់អ្នកដើម្បីសុំជំនួយបន្ទាន់ពេលដែលត្រូវការ ដោយមិនចាំបាច់និយាយដោយត្រង់។&lt;/li&gt;
+    &lt;li&gt;ស្វែងរកមើលថា តើមានជនណាមួយដែលជនប្រព្រឹត្តគោរព និងមានឥទ្ធិពលលើជនប្រព្រឹត្ត ហើយអាចនិយាយជាមួយគេឱ្យឈប់ប្រើអំពើហិង្សា។ ទោះបីជា រយៈពេលខ្លីក៏ដោយ។&lt;/li&gt;
+    &lt;li&gt;កុំនៅស្ងៀម ឬ លាក់បំាង រកសេវាជំនួយពីអាជ្ញាធរមានសមត្ថកិច្ច មន្ត្រីនគរបាល មនុស្សដែលអ្នកជឿ ឬអ្នកដឹកនាំសាសនា ឬអ្នកផ្សេងទៀត។&lt;/li&gt;
+  &lt;/ul&gt;
+&lt;/div&gt;</t>
   </si>
   <si>
     <t>sa_003</t>
@@ -424,7 +763,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -433,6 +772,10 @@
     <font>
       <b/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <name val="Arial"/>
     </font>
     <font>
@@ -445,6 +788,10 @@
       <name val="Nunito"/>
     </font>
     <font>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -472,58 +819,47 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -749,9 +1085,15 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="46.71"/>
-    <col customWidth="1" min="3" max="3" width="51.57"/>
-    <col customWidth="1" min="4" max="4" width="39.0"/>
+    <col customWidth="1" min="1" max="1" width="9.57"/>
+    <col customWidth="1" min="2" max="2" width="35.86"/>
+    <col customWidth="1" min="3" max="3" width="39.57"/>
+    <col customWidth="1" min="4" max="4" width="28.86"/>
+    <col customWidth="1" min="5" max="5" width="12.43"/>
+    <col customWidth="1" min="6" max="6" width="49.86"/>
+    <col customWidth="1" min="8" max="8" width="28.71"/>
+    <col customWidth="1" min="9" max="9" width="29.14"/>
+    <col customWidth="1" min="10" max="10" width="32.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -782,409 +1124,434 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="F3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="F4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="F5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="B6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="F6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="A7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="F7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="A8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="F8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="I9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" ht="36.75" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" ht="37.5" customHeight="1">
+      <c r="A12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C12" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="E12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" ht="108.75" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" ht="51.0" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="A15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" ht="51.75" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="F17" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="A18" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="7" t="b">
+      <c r="A19" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId2"/>
@@ -1205,9 +1572,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="9.57"/>
     <col customWidth="1" min="2" max="2" width="36.0"/>
-    <col customWidth="1" min="3" max="3" width="29.14"/>
+    <col customWidth="1" min="3" max="3" width="44.86"/>
     <col customWidth="1" min="4" max="4" width="45.43"/>
+    <col customWidth="1" min="5" max="5" width="12.43"/>
+    <col customWidth="1" min="6" max="6" width="36.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1234,214 +1604,230 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="A2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" ht="40.5" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" ht="47.25" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" ht="32.25" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" ht="30.75" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" ht="33.0" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" ht="21.75" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" ht="21.0" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" ht="24.75" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="7" t="b">
+      <c r="C13" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="8" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sample data: update content
</commit_message>
<xml_diff>
--- a/lib/samples/assets/csv/categories.xlsx
+++ b/lib/samples/assets/csv/categories.xlsx
@@ -17,7 +17,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="D1">
+    <comment authorId="0" ref="E1">
       <text>
         <t xml:space="preserve">Name must be lowercase and underscore
 	-Sokly Heng</t>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="185">
   <si>
     <t>code</t>
   </si>
@@ -48,6 +48,9 @@
     <t>audio_name</t>
   </si>
   <si>
+    <t>old_audio_name</t>
+  </si>
+  <si>
     <t>parent_code</t>
   </si>
   <si>
@@ -66,6 +69,9 @@
     <t>hint_audio</t>
   </si>
   <si>
+    <t>old_hint_audio</t>
+  </si>
+  <si>
     <t>de_001</t>
   </si>
   <si>
@@ -75,6 +81,9 @@
     <t>before_you_go_prepare_your_trip.png</t>
   </si>
   <si>
+    <t>c1_1_prepare_your_trip.mp3</t>
+  </si>
+  <si>
     <t>prepare_your_trip.mp3</t>
   </si>
   <si>
@@ -84,6 +93,9 @@
     <t>6_thing_before_you_go_hint.png</t>
   </si>
   <si>
+    <t>c1_1_0_six_thing_before_you_go_hint.mp3</t>
+  </si>
+  <si>
     <t>six_thing_before_you_go_hint.mp3</t>
   </si>
   <si>
@@ -96,6 +108,9 @@
     <t>pre_departure_list_passport.png</t>
   </si>
   <si>
+    <t>c1_1_1_passport.mp3</t>
+  </si>
+  <si>
     <t>passport.mp3</t>
   </si>
   <si>
@@ -111,6 +126,9 @@
     <t>pre_departure_list_visa.png</t>
   </si>
   <si>
+    <t>c1_1_2_visa.mp3</t>
+  </si>
+  <si>
     <t>visa.mp3</t>
   </si>
   <si>
@@ -126,130 +144,146 @@
     <t>pre_departure_list_work_permit.png</t>
   </si>
   <si>
+    <t>c1_1_3_work_permit.mp3</t>
+  </si>
+  <si>
     <t>work_permit.mp3</t>
   </si>
   <si>
+    <t>&lt;div&gt;ប័ណ្ណការងារបញ្ជាក់ពីសិទ្ធិរបស់អ្នកក្នុងការធ្វើការងារប្រទេសគោលដៅ។ អ្នកអាចធ្វើប័ណ្ណការងារនេះមុនពេលអ្នកចាកចេញ ឬអាចធ្វើនៅពេលដែលអ្នកទៅដល់ប្រទេសគោលដៅ។&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>de_001_4</t>
+  </si>
+  <si>
+    <t>ប្រភេទនៅមធ្យោបាយធ្វើដំណើរ</t>
+  </si>
+  <si>
+    <t>pre_departure_list_transportation.png</t>
+  </si>
+  <si>
+    <t>c1_1_4_transportation.mp3</t>
+  </si>
+  <si>
+    <t>transportation.mp3</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;ស្គាល់ពីប្រទេសគោលដៅរបស់អ្នក និងប្រភេទមធ្យោបាយដែលអ្នកត្រូវប្រើដើម្បីទៅដល់ប្រទេសគោលដៅ&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>de_001_5</t>
+  </si>
+  <si>
+    <t>ទំនាក់ទំនងជាមួយអ្នកផ្ទះ</t>
+  </si>
+  <si>
+    <t>pre_departure_list_contact_with_home.png</t>
+  </si>
+  <si>
+    <t>c1_1_5_contact_with_home.mp3</t>
+  </si>
+  <si>
+    <t>contact_with_home.mp3</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;វាជាការសំខាន់ណាស់ដែលអ្នកមានលេខទូរស័ព្ទទំនាក់ទំនង និងមធ្យោបាយផ្សេងៗក្នុងការទំនាក់ទំនងអ្នកផ្ទះ ឬមិត្តជិតស្និទ្ធរបស់អ្នក ដែលអាចឱ្យអ្នកផ្តល់ដំណឹងជាទៀងទាត់ពីដំណើររបស់អ្នក។ &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>de_001_6</t>
+  </si>
+  <si>
+    <t>លេខ ឬអាស័យដ្ឋានទំនាក់ទំនង</t>
+  </si>
+  <si>
+    <t>pre_departure_list_contract_address.png</t>
+  </si>
+  <si>
+    <t>c1_1_6_contact_address.mp3</t>
+  </si>
+  <si>
+    <t>contact_address.mp3</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;វាជាការសំខាន់ដែលអ្នកស្គាល់ពីអាស័យដ្ឋាន និងលេខទូរស័ព្ទទំនាក់ទំនងកន្លែងធ្វើការ ឬ/នឹង កន្លែងស្នាក់នៅដើម្បីងាយស្រួលក្នុងការស្វែងរកការគាំទ្រនៅពេលចាំបាច់។&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>de_002</t>
+  </si>
+  <si>
+    <t>ចំណាកស្រុក</t>
+  </si>
+  <si>
+    <t>before_you_go_migration.png</t>
+  </si>
+  <si>
+    <t>c1_2_migration_20.mp3</t>
+  </si>
+  <si>
+    <t>ចំនុចគួររៀបចំសម្រាប់ចំណាកស្រុក</t>
+  </si>
+  <si>
+    <t>5_thing_migration_hint.png</t>
+  </si>
+  <si>
+    <t>c1_2_0_five_thing_migration_hint.mp3</t>
+  </si>
+  <si>
+    <t>five_thing_migration_hint.mp3</t>
+  </si>
+  <si>
+    <t>de_002_1</t>
+  </si>
+  <si>
+    <t>ចាប់ផ្តើមចេញដំណើរ</t>
+  </si>
+  <si>
+    <t>journey_start.png</t>
+  </si>
+  <si>
+    <t>c1_2_1_migration_journey_start.mp3</t>
+  </si>
+  <si>
+    <t>migration_journey_start.mp3</t>
+  </si>
+  <si>
     <t>&lt;div&gt;
-  &lt;h2&gt;៣. ប័ណ្ណការងារ&lt;/h2&gt;
-  &lt;div&gt;ប័ណ្ណការងារបញ្ជាក់ពីសិទ្ធិរបស់អ្នកក្នុងការធ្វើការងារប្រទេសគោលដៅ។ អ្នកអាចធ្វើប័ណ្ណការងារនេះមុនពេលអ្នកចាកចេញ ឬអាចធ្វើនៅពេលដែលអ្នកទៅដល់ប្រទេសគោលដៅ។&lt;/div&gt;
-&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>de_001_4</t>
-  </si>
-  <si>
-    <t>ប្រភេទនៅមធ្យោបាយធ្វើដំណើរ</t>
-  </si>
-  <si>
-    <t>pre_departure_list_transportation.png</t>
-  </si>
-  <si>
-    <t>transportation.mp3</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;ស្គាល់ពីប្រទេសគោលដៅរបស់អ្នក និងប្រភេទមធ្យោបាយដែលអ្នកត្រូវប្រើដើម្បីទៅដល់ប្រទេសគោលដៅ&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>de_001_5</t>
-  </si>
-  <si>
-    <t>ទំនាក់ទំនងជាមួយអ្នកផ្ទះ</t>
-  </si>
-  <si>
-    <t>pre_departure_list_contact_with_home.png</t>
-  </si>
-  <si>
-    <t>contact_with_home.mp3</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;វាជាការសំខាន់ណាស់ដែលអ្នកមានលេខទូរស័ព្ទទំនាក់ទំនង និងមធ្យោបាយផ្សេងៗក្នុងការទំនាក់ទំនងអ្នកផ្ទះ ឬមិត្តជិតស្និទ្ធរបស់អ្នក ដែលអាចឱ្យអ្នកផ្តល់ដំណឹងជាទៀងទាត់ពីដំណើររបស់អ្នក។ &lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>de_001_6</t>
-  </si>
-  <si>
-    <t>លេខ ឬអាស័យដ្ឋានទំនាក់ទំនង</t>
-  </si>
-  <si>
-    <t>pre_departure_list_contract_address.png</t>
-  </si>
-  <si>
-    <t>contact_address.mp3</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;វាជាការសំខាន់ដែលអ្នកស្គាល់ពីអាស័យដ្ឋាន និងលេខទូរស័ព្ទទំនាក់ទំនងកន្លែងធ្វើការ ឬ/នឹង កន្លែងស្នាក់នៅដើម្បីងាយស្រួលក្នុងការស្វែងរកការគាំទ្រនៅពេលចាំបាច់។&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>de_002</t>
-  </si>
-  <si>
-    <t>ចំណាកស្រុក</t>
-  </si>
-  <si>
-    <t>before_you_go_migration.png</t>
-  </si>
-  <si>
-    <t>ចំនុចគួររៀបចំសម្រាប់ចំណាកស្រុក</t>
-  </si>
-  <si>
-    <t>5_thing_migration_hint.png</t>
-  </si>
-  <si>
-    <t>five_thing_migration_hint.mp3</t>
-  </si>
-  <si>
-    <t>de_002_1</t>
-  </si>
-  <si>
-    <t>ចាប់ផ្តើមចេញដំណើរ</t>
-  </si>
-  <si>
-    <t>journey_start.png</t>
-  </si>
-  <si>
-    <t>migration_journey_start.mp3</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;
   &lt;div style='display: flex; flex-direction: row'&gt;
     &lt;div style='width: 120px;'&gt;អ្នកអត្ថាធិប្បាយ៖&lt;/div&gt;
-    &lt;div style='flex: 1'&gt;
-      សួស្តីបងប្អូនដែលជា អ្នកគំាទ្រអ៊ែប (Fan App) """"ដំណើរឆ្លងដែនរបស់ខ្ញុំ។ យើងសង្ឃឹមថាមកដល់ពេលនេះបងប្អូនបានរៀបចំឯកសារពាក់ព័ន្ធរួចរាល់ និងត្រៀមសម្រាប់ការចេញដំណើរនាពេលដ៏ខ្លីខាងមុខនេះ។  ការធ្វើដំណើរ និងឆ្លងដែន គឺជាផ្នែកសំខាន់មួយនៅក្នុងដំណើរចំណាកស្រុក។
-      &lt;p&gt;សូមស្តាប់នូវការសន្ទនាខាងក្រោមនេះ អំពីបទពិសោធឆ្លងដែនរបស់កុលាបដើម្បីស្វែងរកការងារធ្វើនៅក្រៅប្រទេស។&lt;/p&gt;
+    &lt;div style='flex: 1'&gt;សួស្តី​បង​ប្អូន​ដែល​ជា​ អ្នក​គំាទ្រ​អ៊ែប​ (Fan App) ដំណើរ​ឆ្លង​ដែន​របស់​ខ្ញុំ។ យើង​សង្ឃឹម​ថាមក​ដល់​ពេល​នេះ​បង​ប្អូន​បាន​រៀបចំ​ឯកសារ​ពាក់ព័ន្ធ​រួច​រាល់​ និង​ត្រៀម​សម្រាប់​ការ​ចេញ​ដំណើរ​នា​ពេល​ដ៏​ខ្លី​ខាង​មុខ​នេះ។​  ការ​ធ្វើ​ដំណើរ​ និង​ឆ្លង​ដែន​ គឺ​ជា​ផ្នែក​សំខាន់​មួយ​នៅ​ក្នុង​ដំណើរ​ចំណាក​ស្រុក​។
+      &lt;p&gt;សូម​ស្តាប់​នូវ​ការ​សន្ទនា​ខាង​ក្រោម​នេះ​ អំពី​បទពិសោធន៍​ឆ្លង​ដែន​របស់​កុលាប​ដើម្បី​ស្វែង​រក​ការងារ​ធ្វើ​នៅ​ក្រៅ​ប្រទេស។​&lt;/p&gt;
     &lt;/div&gt;
   &lt;/div&gt;
   &lt;div style='display: flex; flex-direction: row'&gt;
-    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;សួស្តី កុលាប! សុខសប្បាយជាទេ?&lt;/div&gt;
-  &lt;/div&gt;
-  &lt;div style='display: flex; flex-direction: row'&gt;
-    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;សួស្តី ម៉ាលីស! អរគុណច្រើន ខ្ញុំសុខសប្បាយជាធម្មតាទេ។&lt;/div&gt;
-  &lt;/div&gt;
-  &lt;div style='display: flex; flex-direction: row'&gt;
-    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ខ្ញុំបានដឹងថាកុលាបធ្លាប់មានបទពិសោធចំណាកស្រុកទៅធ្វើការនៅក្រៅប្រទេស។ និយាយចឹងកុលាបទៅធ្វើការនៅប្រទេសណាដែរ? ទៅតាំងពីពេលណា? ហើយបទពិសោធរបស់កុលាបយ៉ាងម៉េចដែរពេលឆ្លងដែន?&lt;/div&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;សួស្តី កុលាប! សុខ​សប្បាយ​ជា​ទេ?​&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;សួស្តី ម៉ាលីស! អរគុណ​ច្រើន​ ខ្ញុំ​សុខ​សប្បាយ​ជា​ធម្មតា​ទេ។​&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ខ្ញុំ​បាន​ដឹង​ថា​កុលាប​ធ្លាប់​មាន​បទ​ពិសោធន៍​ចំណាក​ស្រុក​ទៅ​ធ្វើ​ការ​នៅ​ក្រៅ​ប្រទេស។​ និយាយ​ចឹង​កុលាប​ទៅ​ធ្វើ​ការ​នៅ​ប្រទេស​ណា​ដែរ?​ ទៅ​តាំង​ពី​ពេល​ណា?​ ហើយ​បទពិសោធន៍​របស់​កុលាប​យ៉ាង​ម៉េច​ដែរ​ពេល​ឆ្លង​ដែន?​&lt;/div&gt;
   &lt;/div&gt;
   &lt;div style='display: flex; flex-direction: row'&gt;
     &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;
     &lt;div style='flex: 1'&gt;
-      &lt;div&gt;ខ្ញុំទៅធ្វើការនៅប្រទេសថៃ ប្រហែលជាងពីរឆ្នាំហើយ ខ្ញុំទើបមកស្រុកវិញបានប្រមាណជាងពីរអាទិត្យហ្នឹង។&lt;/div&gt;
-      &lt;p&gt;ហូ៎ ពេលបួនប្រាំថ្ងៃមុនពេលចេញដំណើរ ខ្ញុំបានសួរបងស្រីជីដូនមួយខ្ញុំដែលធ្លាប់ទៅធ្វើការនៅថៃ និងស្វែងយល់ព័ត៌មានបន្ថែមពីអ្វីដែលត្រូវការសម្រាប់ឆ្លងដែន តាមរយៈហេ្វសបុកផ្លូវការរបស់ក្រសួង និងអង្គការសង្គមស៊ីវិលមានការងារពាក់ព័ន្ធចំណាកស្រុក ស្តាប់វិទ្យុ និងខិតបណ្ណ័ផ្សព្វផ្សាយទាក់ទងនឹងចំណាកស្រុកនានា។&lt;/p&gt;
+      &lt;div&gt;ខ្ញុំ​ទៅ​ធ្វើ​ការ​នៅ​ប្រទេស​ថៃ​ ប្រហែល​ជាង​ពីរ​ឆ្នាំ​ហើយ​ ខ្ញុំ​ទើប​មក​ស្រុក​វិញ​បាន​ប្រមាណ​ជាង​ពីរ​អាទិត្យ​ហ្នឹង។​&lt;/div&gt;
+      &lt;p&gt;ហូ៎​ ពេល​បួនប្រាំ​ថ្ងៃ​មុន​ពេល​ចេញ​ដំណើរ​ ខ្ញុំ​បាន​សួរ​បង​ស្រី​ជី​ដូន​មួយ​ខ្ញុំ​ដែល​ធ្លាប់​ទៅ​ធ្វើ​ការ​នៅ​ថៃ​ និង​ស្វែង​យល់​ព័ត៌មាន​បន្ថែម​ពី​អ្វី​ដែល​ត្រូវ​ការ​សម្រាប់​ឆ្លង​ដែន​ តាម​រយៈ​ហេ្វសបុក​ផ្លូវ​ការ​របស់​ក្រសួង​ និង​អង្គការ​សង្គម​ស៊ីវិល​មាន​ការងារ​ពាក់​ព័ន្ធ​ចំណាក​ស្រុក​ ស្តាប់​វិទ្យុ​ និង​ខិត​បណ្ណ័​ផ្សព្វផ្សាយ​ទាក់​ទង​នឹង​ចំណាក​ស្រុក​នានា។​&lt;/p&gt;
       &lt;p&gt;ម៉ាលីសឯងចង់ទៅធ្វើការនៅប្រទេសគេមែនទេ? អញ្ចឹងម៉ាលីសត្រូវតែមានលិខិតឆ្លងដែនទិដ្ឋាការ(វីសា) និងឯកសារការងារ ឬប័ណ្ណការងារ ទើបគេអនុញ្ញាត្តិឲ្យយើងចូលប្រទេសគេដើម្បីធ្វើការ វាគឺជាតម្រូវការចំាបាច់។ កាលនោះ ខ្ញុំបានរៀបចំទុកដាក់លិខិតឆ្លងដែន ឯកសារសំខាន់ៗ លុយកាក់ និងរបស់របរប្រើប្រាស់ចាំបាច់ ដូចជាសំឡីអនាម័យ ប្រេងកូឡា ឬប្រេងខ្យល់នៅក្នុងកាបូបស្ពាយជាប់ខ្លួនដើម្បីងាយស្រួលរកពេលត្រូវការបន្ទាន់។ ខ្ញុំមិនដាក់នៅក្នុងកាតាបដាក់ខោអាវ និងគ្រឿងប្រើប្រាស់ទូទៅនោះទេ ព្រោះពេលធ្វើដំណើរកាតាបនោះមិននៅក្បែរយើងទេ។&lt;/p&gt;
-      &lt;p&gt;នៅពេលដែលយើងធ្វើដំណើរដល់ព្រំដែន យើងត្រូវបំពេញលិខិតចេញពីខាងប្រទេសយើង និងលិខិតចូលទៅខាងប្រទេសគេ។ លិខិតហ្នឹង គឹយើងត្រូវបំពេញព័ត៌មានឲ្យបានត្រឹមត្រូវ ដូចជាឈ្មោះបុគ្គល ឬឈ្មោះទីកន្លែង និងលេខទូរសព្ទ័ដែលយើងត្រូវទៅក្នុងប្រទេសថៃ។&lt;/p&gt;
-      &lt;p&gt;តាមខ្ញុំដឹង នៅពេលយើងចូលទៅប្រទេសណាក៏ដោយ ក៏ត្រូវបំពេញលិខិតចូលដែរ វាជាលក្ខខណ្ឌមិនអាចខ្វះបាន ទោះជិះឡាន ឬយន្តហោះ។&lt;/p&gt;
+      &lt;p&gt;នៅ​ពេល​ដែល​យើង​ធ្វើ​ដំណើរ​ដល់​ព្រំដែន​ យើង​ត្រូវ​បំពេញ​លិខិត​ចេញ​ពី​ខាង​ប្រទេស​យើង​ និង​លិខិត​ចូល​ទៅ​ខាង​ប្រទេស​គេ។​ លិខិត​ហ្នឹង​ គឹ​យើង​ត្រូវ​បំពេញ​ព័ត៌មាន​ឲ្យ​បាន​ត្រឹម​ត្រូវ​ ដូច​ជាឈ្មោះ​បុគ្គល​ ឬឈ្មោះ​ទី​កន្លែង​ និង​លេខ​ទូរសព្ទ័​ដែល​យើង​ត្រូវ​ទៅ​ក្នុង​ប្រទេស​ថៃ។​&lt;/p&gt;
+      &lt;p&gt;តាម​ខ្ញុំ​ដឹង​ នៅ​ពេល​យើង​ចូល​ទៅ​ប្រទេស​ណា​ក៏​ដោយ​ ក៏​ត្រូវ​បំពេញ​លិខិត​ចូល​ដែរ​ វា​ជា​លក្ខខណ្ឌ​មិន​អាច​ខ្វះ​បាន​ ទោះ​ជិះ​ឡាន​ ឬ​យន្ត​ហោះ។​&lt;/p&gt;
     &lt;/div&gt;
   &lt;/div&gt;
   &lt;div style='display: flex; flex-direction: row'&gt;
     &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ហូ៎ អីចឹងផង! ខ្ញុំមិនដែលដឹងសោះ។&lt;/div&gt;
   &lt;/div&gt;
   &lt;div style='display: flex; flex-direction: row'&gt;
-    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ម៉ាលីសដឹងទេ  ចំពោះបទពិសោធន៍ខ្ញុំ ខ្ញុំគិតថាសំខាន់ខ្លាំងណាស់ដែលយើងធ្វើដំណើរជាមួយអ្នកដែលយើងស្គាល់ច្បាស់បំផុត អាចជាបងប្អូន ពូមីង ឬអ្នកនៅក្នុងភូមិដែលយើងស្គាល់ប្រវត្តិរបស់គេត្រឹមត្រូវ ព្រោះថានាំឲ្យខ្ញុំមានភាពកក់ក្តៅ នៅពេលមានអ្នករួមដំណើរដែលអាចជឿទុកចិត្តបាន។&lt;/div&gt;
-  &lt;/div&gt;
-  &lt;div style='display: flex; flex-direction: row'&gt;
-    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ពិតមែនហើយ ពេលទៅជាមួយអ្នកស្គាល់ និងជឿទុកចិត្ត គឺអាចជួយគ្នាបាន។ ចុះពេលកុលាបធ្វើដំណើរយូរទេពីភូមិយើងទៅដល់ទល់ដែន ប្រហែលជាប៉ុន្មានម៉ោង? ជិះទៅអស់លុយប្រហែលប៉ុន្មាន?&lt;/div&gt;
-  &lt;/div&gt;
-  &lt;div style='display: flex; flex-direction: row'&gt;
-    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;
-      ជិះពីភូមិយើង (ស្រុកបរសេដ្ឋ ខេត្តកំពង់ស្ពី) ទៅដល់ព្រំដែនឡែមដែលខ្ញុំឆ្លងហ្នឹង ប្រហែលជាង ៥ ទៅ ៦ ម៉ោង ព្រោះយើងមានឈប់ខ្លះ ចូលបន្ទប់ទឹក និងញាំអាហារ។  ពីភូមិទៅដល់ព្រំដែនម្នាក់អស់ប្រហែលជាង ៤ ម៉ឺនរៀល ហើយពីព្រំដែនទៅដល់គោលដៅ ជិះប្រហែលជាងពីរម៉ោងទៀត និងអស់ថ្លៃជិះចន្លោះពី ១៥០បាត ទៅ ២០០ បាត។ តាមបទពិសោធខ្ញុំ យើងគួរតែទាក់ទងឲ្យដឹងឡានណា ចេញម៉ោងប៉ុន្មាន? ចេញដំណើរពីទីតាំងណា? តើឡានហ្នឹងទៅដល់ទល់ដែនតែម្តង ឬយ៉ាងណា?
-      &lt;p&gt;បើយើងទៅជាក្រុម យើងគួរទាក់ទងគ្នាកំណត់ម៉ោងពេលចេញដំណើរឲ្យបានច្បាស់ដូចគ្នា យើងគួរតែដឹងពីទីតាំងឡានចេញដំណើរ និងគោលដៅដែលឡាននឹងឈប់ផងដែរ។&lt;/p&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ម៉ាលីស​ដឹង​ទេ​  ចំពោះ​បទ​ពិសោធន៍​ខ្ញុំ​ ខ្ញុំ​គិត​ថា​សំខាន់​ខ្លាំង​ណាស់​ដែល​យើង​ធ្វើ​ដំណើរ​ជា​មួយ​អ្នក​ដែល​យើង​ស្គាល់​ច្បាស់​បំផុត​ អាច​ជា​បង​ប្អូន​ ពូ​មីង​ ឬ​អ្នក​នៅ​ក្នុង​ភូមិ​ដែល​យើង​ស្គាល់​ប្រវត្តិ​របស់​គេ​ត្រឹម​ត្រូវ​ ព្រោះ​ថា​នាំ​ឲ្យ​ខ្ញុំ​មាន​ភាព​កក់ក្តៅ​ នៅ​ពេល​មាន​អ្នក​រួម​ដំណើរ​ដែល​អាច​ជឿ​ទុក​ចិត្ត​បាន។​&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ពិត​មែន​ហើយ​ ពេល​ទៅ​ជា​មួយ​អ្នក​ស្គាល់​ និង​ជឿ​ទុក​ចិត្ត​ គឺ​អាច​ជួយ​គ្នា​បាន។​ ចុះ​ពេល​កុលាប​ធ្វើ​ដំណើរ​យូរ​ទេ​ពី​ភូមិ​យើង​ទៅ​ដល់​ទល់​ដែន​ ប្រហែល​ជា​ប៉ុន្មាន​ម៉ោង?​ ជិះ​ទៅ​អស់​លុយ​ប្រហែល​ប៉ុន្មាន?​&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ជិះ​ពី​ភូមិ​យើង​ (ស្រុក​បរសេដ្ឋ​ ខេត្ត​កំពង់​ស្ពី​) ទៅ​ដល់​ព្រំដែន​ឡែម​ដែល​ខ្ញុំ​ឆ្លង​ហ្នឹង​ ប្រហែល​ជាង​ ៥ ទៅ​ ៦ ម៉ោង​ ព្រោះ​យើង​មាន​ឈប់​ខ្លះ​ ចូល​បន្ទប់​ទឹក​ និង​ញាំ​អាហារ។​  ពី​ភូមិ​ទៅ​ដល់​ព្រំ​ដែន​ម្នាក់​អស់​ប្រហែល​ជាង​ ៤ ម៉ឺន​រៀល​ ហើយ​ពី​ព្រំដែន​ទៅ​ដល់​គោលដៅ​ ជិះ​ប្រហែល​ជាង​ពីរ​ម៉ោង​ទៀត​ និង​អស់​ថ្លៃ​ជិះ​ចន្លោះ​ពី​ ១៥០បាត​ ទៅ​ ២០០ បាត។​ តាម​បទពិសោធន៍​ញុំ​ យើង​គួរ​តែ​ទាក់ទង​ឲ្យ​ដឹង​ឡាន​ណា​ ចេញ​ម៉ោង​ប៉ុន្មាន?​ ចេញ​ដំណើរ​ពី​ទីតាំង​ណា?​ តើ​ឡាន​ហ្នឹង​ទៅ​ដល់​ទល់​ដែន​តែ​ម្តង​ ឬ​យ៉ាង​ណា?​
+      &lt;p&gt;បើ​យើង​ទៅ​ជា​ក្រុម​ យើង​គួរ​ទាក់​ទង​គ្នា​កំណត់​ម៉ោង​ពេល​ចេញ​ដំណើរ​ឲ្យ​បាន​ច្បាស់​ដូច​គ្នា​ យើង​គួរ​តែ​ដឹង​ពី​ទី​តាំង​ឡាន​ចេញ​ដំណើរ​ និង​គោល​ដៅ​ដែល​ឡាន​នឹង​ឈប់​ផង​ដែរ។​&lt;/p&gt;
     &lt;/div&gt;
   &lt;/div&gt;
   &lt;div style='display: flex; flex-direction: row'&gt;
@@ -259,7 +293,7 @@
     &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;អូ៎ ម៉ាលីស មុននឹងទៅដល់ទល់ដែន ខ្ញុំប្រាប់បទពិសោធសំខាន់មួយទៀតដល់ម៉ាលីសឯង។ វាពិតជាសំខាន់ណាស់! យើងត្រូវប្រាប់ពុកម៉ែ និងបងប្អូនជិតស្និត អំពីរយៈពេលនៃការធ្វើដំណើររបស់យើង ប្រហែលជាចំណាយអស់ប៉ុន្មានម៉ោង? ទៅដល់ព្រំដែនប្រហែលម៉ោងប៉ុន្មាន? ហើយឆ្លងពីព្រំដែនទៅដល់ទីកន្លែងដែលយើងត្រូវទៅចំណាយអស់ប្រហែលប៉ុន្មានម៉ោង? អូ៎មួយទៀត លេខទូរស័ព្ទទំនាក់ទំនងរបស់សាច់ញាត្តិជិតស្និតរបស់យើងក៏គួរចំា ឬកត់ត្រាទុក ដែលយើងអាចរកបានភ្លាមៗផងដែរ ពេលយើងជួបបញ្ហាបន្ទាន់ ឬពេលត្រូវការប្រើចាំបាច់។&lt;/div&gt;
   &lt;/div&gt;
   &lt;div style='display: flex; flex-direction: row'&gt;
-    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;អរគុណសម្រាប់ការចែករំលែកបទពិសោធក្នុងការធ្វើដំណើរ។ ស្តាប់មើលទៅ គឺសំខាន់ណាស់! ចុះពេលទៅដល់ទល់ដែន កុលាបឯងមានបទពិសោធម៉េចដែរ?&lt;/div&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;អរគុណសម្រាប់ការចែករំលែកបទពិសោធន៍ក្នុងការធ្វើដំណើរ។ ស្តាប់មើលទៅ គឺសំខាន់ណាស់! ចុះពេលទៅដល់ទល់ដែន កុលាបឯងមានបទពិសោធន៍ម៉េចដែរ?&lt;/div&gt;
   &lt;/div&gt;
   &lt;div style='display: flex; flex-direction: row'&gt;
     &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;នៅច្រកទល់ដែន គឺមានសកម្មភាពចេញចូលជាហូរហែរ មានការដឹកជញ្ជូនទំនិញ និងមនុស្សឆ្លងកាត់។ ហើយការឆ្លងកាត់ទាំងនោះ មិនមែនចេញចូលស្រេចតែចិត្តនោះទេ ម៉ាលីសអើយ សុទ្ធតែឆ្លងកាត់ការត្រួតពិនិត្យពីខាងប្រទេសយើង បោះត្រាចេញពីខាងមន្ត្រីប៉ូលីសប្រចំាការងារព្រំដែន។ យើងត្រូវរង់ចាំរហូតដល់វេនរបស់យើង ប្រសិនបើមានមនុស្សចេញច្រើន។ ពេលខ្លះ ប៉ូលីសមើលការងារព្រំដែន ក៏សួរយើងមួយ ឬពីរសំនួរផងដែរ តើយើងទៅប្រទេសគេធ្វើអ្វី? ស្នាក់នៅកន្លែងណា?&lt;/div&gt;
@@ -277,7 +311,7 @@
     &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;កាលណុង ខ្ញុំដាក់ទីតាំងស្នាក់នៅជាមួយនឹងបងប្អូនជីដូនមួយខ្ញុំ ដែលគាត់ធ្វើការ និងរស់នៅប្រទេសថៃ ដោយសារគាត់មានទីតាំងជាក់លាក់។&lt;/div&gt;
   &lt;/div&gt;
   &lt;div style='display: flex; flex-direction: row'&gt;
-    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;អរគុណចំពោះការចែករំលែកនូវបទពិសោធ ខ្ញុំបានដឹងច្រើនពីអ្វីដែលកុលាប បានធ្វើដើម្បីឆ្លងដែន។&lt;/div&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;អរគុណចំពោះការចែករំលែកនូវបទពិសោធន៍ ខ្ញុំបានដឹងច្រើនពីអ្វីដែលកុលាប បានធ្វើដើម្បីឆ្លងដែន។&lt;/div&gt;
   &lt;/div&gt;
 &lt;/div&gt;</t>
   </si>
@@ -289,6 +323,9 @@
   </si>
   <si>
     <t>migration_understanding_your_contract.png</t>
+  </si>
+  <si>
+    <t>c1_2_2_migration_understanding_your_contract.mp3</t>
   </si>
   <si>
     <t>migration_understanding_your_contract.mp3</t>
@@ -313,15 +350,18 @@
     <t>migration_worker_right.png</t>
   </si>
   <si>
+    <t>c1_2_3_migration_worker_right.mp3</t>
+  </si>
+  <si>
     <t>migration_worker_right.mp3</t>
   </si>
   <si>
     <t>&lt;div&gt;
   &lt;div&gt;ទោះបីជាស្ថានភាពចំណាកស្រុករបស់អ្នកយ៉ាងណាក៏ដោយ អ្នកត្រូវតែទទួលបានសិទ្ធិ និងការគាំពារពេញលេញដូចខាងក្រោម៖&lt;/div&gt;
   &lt;ul&gt;
-    &lt;li&gt;សេរីភាពរក្សាអត្តសញ្ញាណរបស់ខ្លួន និងឯកសារសំខាន់ៗផ្សេងៗ&lt;/li&gt;
+    &lt;li&gt;សេរីភាព​រក្សា​អត្តសញ្ញាណ​របស់​ខ្លួន​ និង​ឯកសារ​សំខាន់ៗ​ផ្សេងៗ​&lt;/li&gt;
     &lt;li&gt;សេរីភាពចូលរួមក្នុងសមាគមន៍ដូចជា សហជីព និងសមាគមន៍កម្មករ&lt;/li&gt;
-    &lt;li&gt;សេរីភាពរួចផុតពីអំពើហិង្សា និងការបៀតបៀនផ្សេងៗ រួមទាំងការបៀតបៀនផ្លូវភេទទំាងក្នុង និងក្រៅកន្លែងការងារ&lt;/li&gt;
+    &lt;li&gt;សេរីភាព​រួច​ផុត​ពី​អំពើ​ហិង្សា​ និង​ការ​បៀត​បៀន​ផ្សេងៗ​ ​រួម​ទាំង​ការ​បៀត​បៀន​ផ្លូវ​ភេទ​ទំាង​ក្នុង​ និង​ក្រៅ​កន្លែង​ការងារ​&lt;/li&gt;
     &lt;li&gt;សិទ្ធិតវ៉ា និងដាក់ពាក្យបណ្តឹងពីបញ្ហានៅកន្លែងការងារ&lt;/li&gt;
   &lt;/ul&gt;
 &lt;/div&gt;</t>
@@ -336,6 +376,9 @@
     <t>culture_and_living.png</t>
   </si>
   <si>
+    <t>c1_2_4_migration_calture_and_living.mp3</t>
+  </si>
+  <si>
     <t>migration_calture_and_living.mp3</t>
   </si>
   <si>
@@ -365,13 +408,16 @@
     <t>money_saving_tip.png</t>
   </si>
   <si>
+    <t>c1_2_5_migration_saving_tip.mp3</t>
+  </si>
+  <si>
     <t>migration_saving_tip.mp3</t>
   </si>
   <si>
     <t>&lt;div&gt;
-  &lt;div&gt;ការសន្សំប្រាក់ពិតជាសំខាន់ខ្លាំងណាស់! ប្រាក់សន្សំរួមចំណែកធ្វើអោយការចំណាកស្រុករបស់អ្នកទទួលបានជោគជ័យ។ ការសន្សំប្រាក់ជួយអោយអ្នកសម្រេចគោលបំណង ដូចជាការបង្កើតមុខរបរ ឬរៀនជំនាញជាក់លាក់សម្រាប់ខ្លួនឯងពេលត្រលប់មកស្រុកវិញ ព្រមទំាងជួយស្តារស្ថានភាព ឬជីវភាពគ្រួសារ ប្រើប្រាស់ក្នុងគ្រាអាសន្នណាមួយ និងជួយគាំទ្រការសិក្សាកូនៗ។&lt;/div&gt;
-  &lt;p&gt;ប្រាក់សន្សំ ជាប្រាក់ដែលអ្នកទុកដាច់ដោយឡែកក្រោយពីទូទាត់រាល់ការចំណាយទាំងអស់ ដូចជា ការបង់ថ្លៃផ្ទះ ឬបន្ទប់ជួល ថ្លៃទឹកភ្លើង ការចំណាយលើម្ហូបអាហារប្រចាំថ្ងៃ និងការចំណាយចំាបាច់ផ្សេងៗ ព្រមទំាងប្រាក់ផ្ញើត្រឡប់មកផ្ទះផងដែរ។&lt;/p&gt;
-  &lt;p&gt;អ្នកអាចរៀបចំផែនការសន្សំប្រាក់របស់អ្នកដោយគិតលើទឹកប្រាក់ដែលអ្នកចង់ទទួលបានធៀបនឹងរយៈពេលនៃការសន្សំរបស់អ្នក។ ឧទាហរណ៌ អ្នកចង់បានប្រាក់ ៦០០ដុល្លារក្នុងរយៈពេលពីរឆ្នាំ ដូចនេះអ្នកត្រូវដកទុកចំនួន ២៥ដុល្លារ ក្នុងមួយខែជាប្រចាំ។​ អ្នកអាចទុកដាក់លុយនៅកន្លែងដែលអ្នកគិតថាមានសុវត្ថិភាពបំផុត ដូចជា ប្រអប់សុវត្ថិភាព រឺបើកគណនីសន្សំនៅធនាគារណាមួយ។&lt;/p&gt;
+  &lt;div&gt;ការ​សន្សំ​ប្រាក់​ពិត​ជា​សំខាន់ខ្លាំង​ណាស់!​ ប្រាក់​សន្សំ​រួម​ចំណែក​ធ្វើ​អោយ​ការ​ចំណាក​ស្រុក​របស់​អ្នក​ទទួល​បាន​ជោគជ័យ។​ ការ​សន្សំ​ប្រាក់​ជួយ​អោយ​អ្នក​សម្រេច​គោល​បំណង​ ដូច​ជា​ការ​បង្កើត​មុខ​របរ​ ឬ​រៀន​ជំនាញ​ជាក់​លាក់​សម្រាប់​ខ្លួន​ឯង​ពេល​ត្រលប់​មក​ស្រុក​វិញ​ ព្រម​ទំាង​ជួយ​ស្តារ​ស្ថាន​ភាព​ ឬ​ជីវភាព​គ្រួសារ​ ប្រើ​ប្រាស់​ក្នុង​គ្រា​អាសន្ន​ណា​មួយ​ និង​ជួយ​គាំទ្រ​ការ​សិក្សា​កូនៗ។​&lt;/div&gt;
+  &lt;p&gt;ប្រាក់​សន្សំ​ ជា​ប្រាក់​ដែល​អ្នក​ទុក​ដាច់​ដោយ​ឡែក​ក្រោយ​ពី​ទូទាត់​រាល់​ការ​ចំណាយ​ទាំង​អស់​ ដូច​ជា​ ការ​បង់​ថ្លៃ​ផ្ទះ​ ឬ​បន្ទប់​ជួល​ ថ្លៃ​ទឹក​ភ្លើង​ ការ​ចំណាយ​លើ​ម្ហូប​អាហារ​ប្រចាំ​ថ្ងៃ​ និង​ការ​ចំណាយ​ចំា​បាច់​ផ្សេងៗ​ ព្រម​ទំាង​ប្រាក់​ផ្ញើ​ត្រឡប់​មក​ផ្ទះ​ផង​ដែរ។​&lt;/p&gt;
+  &lt;p&gt;អ្នក​អាច​រៀប​ចំ​ផែន​ការ​សន្សំ​ប្រាក់​របស់​អ្នក​ដោយ​គិត​លើ​ទឹក​ប្រាក់​ដែល​អ្នក​ចង់​ទទួល​បាន​ធៀប​នឹង​រយៈ​ពេល​នៃ​ការ​សន្សំ​របស់​អ្នក។​ ឧទាហរណ៌​ អ្នក​ចង់​បាន​ប្រាក់​ ៦០០​ដុល្លារ​ក្នុង​រយៈ​ពេល​ពីរ​ឆ្នាំ​ ដូច​នេះ​អ្នក​ត្រូវ​ដក​ទុក​ចំនួន​ ២៥ដុល្លារ​ ក្នុង​មួយ​ខែ​ជា​ប្រចាំ។​​ អ្នក​អាច​ទុក​ដាក់​លុយ​នៅ​កន្លែង​ដែល​អ្នក​គិត​ថា​មាន​សុវត្ថិភាព​បំផុត​ ដូច​ជា​ ប្រអប់​សុវត្ថិភាព​ រឺ​បើក​គណនី​សន្សំ​នៅ​ធនាគារ​ណា​មួយ។​&lt;/p&gt;
 &lt;/div&gt;</t>
   </si>
   <si>
@@ -384,12 +430,18 @@
     <t>before_you_go_coming_home.png</t>
   </si>
   <si>
+    <t>c1_3_retruning_trip.mp3</t>
+  </si>
+  <si>
     <t>ចំនុចដើម្បីរៀបចំវិលត្រលប់មកស្រុកវិញ</t>
   </si>
   <si>
     <t>3_things_coming_home_hint.png</t>
   </si>
   <si>
+    <t>c1_3_0_three_thing_coming_home_hint.mp3</t>
+  </si>
+  <si>
     <t>three_thing_coming_home_hint.mp3</t>
   </si>
   <si>
@@ -400,6 +452,9 @@
   </si>
   <si>
     <t>coming_home_make_your_plan.png</t>
+  </si>
+  <si>
+    <t>c1_3_1_coming_home_prepare_plan.mp3</t>
   </si>
   <si>
     <t>coming_home_prepare_plan.mp3</t>
@@ -444,6 +499,9 @@
     <t>coming_home_women_migrant_worker.png</t>
   </si>
   <si>
+    <t>c1_3_2_coming_home_back_home.mp3</t>
+  </si>
+  <si>
     <t>coming_home_back_home.mp3</t>
   </si>
   <si>
@@ -459,6 +517,33 @@
     <t>coming_home_women_migrant_worker_and_economic.png</t>
   </si>
   <si>
+    <t>c1_3_3_coming_home_women_migrant_worker_and_economic.mp3</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;
+&lt;div&gt;ស្វែងយលពីស្ត្រី និងការចំណាកស្រុកសុវត្ថិភាព&lt;/div&gt;
+&lt;div&gt;ការធ្វើទេសន្តរប្រវេសន៍ អាចផ្តល់នូវប្រយោជន៍គ្រប់តួអង្គពាក់ព័ន្ធទាំងអស់។ ពលករទេសន្តរប្រវេសន៍ជាស្ត្រី រួមភាគទានផ្នែកសង្គម និងសេដ្ឋកិច្ចយ៉ាងសំខាន់ដល់សហគមន៍របស់ពួកគេ ក៏ដូចជាដល់ប្រទេសប្រភពដើម និងប្រទេសគោលដៅ។ ស្ត្រីដែលធ្វើទេសន្តរប្រវេសន៍ អាចទទួលបានការងារដែលផ្តល់នូវប្រាក់កំរៃខ្ពស់ ហើយក្នុងពេលជាមួយគ្នា អាចបង្កើនភាពជាតំណាងរបស់ពួកគេ ក៏ដូចជាធ្វើអោយស្ថានភាពក្នុងគ្រួសារ និងសហគមន៍របស់ពួកគេ កាន់តែមានភាពល្អប្រសើរជាងមុន ដូច្នេះទេសន្តរប្រវេសន៍ការងាររបស់ស្ត្រី អាចជាប្រភពដ៏សំខាន់ សម្រាប់ផ្តល់ភាពអង្គអាចដល់ស្ត្រី។ មានការប៉ាន់ប្រមាណថា នៅក្នុងឆ្នាំ ២០១៦ ប្រាក់ដែលបញ្ជូនដោយពលករទេសន្តរប្រវេសន៍ មកប្រទេសកំណើតរបស់ពួកគេមានចំនួន 63.9 ពាន់លានដុល្លា ប្រហែលជាពាក់កណ្តាលនៃប្រាក់នេះ ត្រូវបានបញ្ជូនត្រឡប់ដោយស្ត្រី។ ទោះជាយ៉ាងណាក៏ដោយ នៅក្នុងវដ្ដនៃការធ្វើទេសន្តរប្រវេសន៍ ពលករទេសន្តរប្រវេសន៍ជាស្ត្រីប្រឈមនឹងអំពើហិង្សា ការជួញដូរមនុស្ស និងការរើសអើងដែលរឹតត្បឹតលទ្ធភាពរបស់ពួកគេមិនអោយ ទទួលបានការជ្រើសរើសធ្វើជាពលករដោយ យុត្តិធម៌ និងការងារសមរម្យ។ ពួកគេក៏មានឱកាសតិចតួច ក្នុងការទទួលបានសេវាការពារ និងគាំទ្រផងដែរ។ &lt;/div&gt;
+&lt;div&gt;តើអ្វីជាការចំណាកស្រុកប្រកបដោយសុវត្ថិភាព 
+ការចំណាកស្រុកគឺជាការ បំលាស់ទីរបស់មនុស្សម្នាក់ ឬមនុស្សមួយក្រុមឆ្លងប្រទេស ឬនៅក្នុងប្រទេសដោយមូលហេតុផ្សេងៗគ្នា។ &lt;/div&gt;
+&lt;div&gt;ចំណាកស្រុកដោយសុវត្ថិភាព គឺសំដៅដល់ការចំណាកស្រុកដែលមានឯកសារស្របច្បាប់ ឬហៅថាចំណាកស្រុកស្របច្បាប់។ &lt;/div&gt;
+&lt;div&gt;ភាពខុសគ្នារវាង ចំណាកស្រុកស្របច្បាប់ និងចំណាកស្រុកខុសច្បាប់។&lt;/div&gt;
+&lt;div&gt;ចំណាកស្រុកស្របច្បាប់មានឯកសារស្របច្បាប់ដូចជា លិខិតឆ្លងដែន ទិដ្ឋិការ លិខិតអនុញ្ញាតិអោយធ្វើការពីក្រសួងការងារ កិច្ចសន្យាការងារ ទាំងអស់នោះអាចអោយអ្នកមានការងារ សុវត្ថិភាព ជាក់លាក់ហើយអាចចៀសផុតពីអំពើជួញដូរមនុស្ស អំពើកេងប្រវ័ញ្ច និងសុវត្ថិភាពពេលអ្នកធ្វើដំណើរ។&lt;/div&gt;
+&lt;div&gt;ការចំណាកស្រុកខុសច្បាប់ គឺមិនមានឯកសារស្របច្បាប់ ដោយធ្វើការចំណាកស្រុកតាមរយៈមេខ្យល់ សាច់ញាតិ មិត្តភក្តិ  អ្នកដែលមិនស្គាល់គ្នា ឆ្លងកាត់ព្រំដែនដោយខ្លួនឯង និងនាំអោយអ្នកអាចជួបគ្រោះថ្នាក់ ពេលកំពុងធ្វើដំណើរ ប្រឈមភាពគ្មានការងារធ្វើ និងកាន់តែងាយត្រូវបានគេជួញដូរ និងកេងប្រវ័ញ្ច។&lt;/div&gt;
+&lt;div&gt;ដើម្បីអោយអាចធ្វើចំណាកស្រុកសុវត្ថិភាព អ្នកគួរពិចារណានូវចំនុចមួយចំនួនដូចខាងក្រោម៖&lt;/div&gt;
+&lt;ol&gt;
+&lt;li&gt;តើខ្ញុំមានអត្តសញ្ញាណប័ណ្ណ ឬលិខិតឆ្លងដែនដែលមានសុពលភាពឬទេ?&lt;/li&gt;
+&lt;li&gt;តើប្រទេសដែលខ្ញុំចង់ទៅ ត្រូវការទិដ្ឋការសម្រាប់ស្នាក់នៅ និងធ្វើការរយៈពេលវែងដែរឬទេ?&lt;/li&gt;
+&lt;li&gt;តើខ្ញុំត្រូវការដឹងនូវអ្វីខ្លះ មុននឹងសម្រេចចិត្ត វប្បធ៌ម ការរស់នៅរបស់ប្រទេសគោលដៅមានសភាពយ៉ាងដូចម្តេច?&lt;/li&gt;
+&lt;li&gt;តើខ្ញុំត្រូវទាក់ទងទៅអ្នកណា ពេលខ្ញុំត្រូវការជំនួយបន្ទាន់?&lt;/li&gt;
+&lt;li&gt;ក្នុងពេលដែលអ្នកសម្រេចចាកចេញពីកន្លែងស្នាក់នៅ ឬធ្វើការជាបន្ទាន់ តើអ្នកត្រូវធ្វើដូចម្តេច?
+(កញ្ចប់ត្រៀមបង្ការមានដូចជា អត្តសញ្ញាណប័ណ្ណ ឬលិខិតឆ្លងដែន លុយកាក់មួយចំនួន កាតទូរស័ព្ទ និងសម្ភារៈចាំបាច់ផ្សេងៗទៀតគួរតែមានរៀបចំទុកជាស្រេច)&lt;/li&gt;
+&lt;li&gt;នៅពេលខ្ញុំមិនទាន់ចង់មានផ្ទៃពោះ តើខ្ញុំត្រូវធ្វើដូចម្តេច? (ស្រោមអនាម័យគឺជាមធ្យោបាយតែមួយគត់ ដើម្បីការពារពីការមានផ្ទៃពោះមិនចង់បាន និងការឆ្លងមេរោគអេដស៍)&lt;/li&gt;
+&lt;li&gt;ការបៀតបៀនផ្លូវភេទមិនមែនជាកំហុសរបស់ស្ត្រីទេ ផ្ទុយទៅវិញ វាជាបញ្ហារបស់អ្នកប្រព្រឹត្ត និងកង្វះខាតពីការគិតគូរ មិនអោយមានពីការបៀតបៀនផ្លូវភេទលើស្ត្រី នៅកន្លែងសាធារណៈ។&lt;/li&gt;
+&lt;li&gt;តើខ្ញុំមានលេខទូរស័ព្ទទំនាក់ទំនងសាច់ញាតិ ឬមនុស្សដែលខ្ញុំទុកចិត្តដែរឬទេ? តើមានលេខទូរស័ព្ទសង្គ្រោះបន្ទាន់ ដូចជាអង្គការមិនមែនរដ្ឋាភិបាល នគរបាល ស្ថានទូត ភ្នាក់ងារផ្តល់សេវាសុខភាពនៅក្នុងប្រទេសគោលដៅ ដែលខ្ញុំអាចស្វែងរកជំនួយបានដែរឬទេ? &lt;/li&gt;
+&lt;/ol&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>de_004</t>
   </si>
   <si>
@@ -468,6 +553,9 @@
     <t>before_you_go_video.png</t>
   </si>
   <si>
+    <t>video.mp3</t>
+  </si>
+  <si>
     <t>sa_001</t>
   </si>
   <si>
@@ -477,6 +565,9 @@
     <t>your_safety_safety_planning.png</t>
   </si>
   <si>
+    <t>c2_1_right_and_your_safety.mp3</t>
+  </si>
+  <si>
     <t>right_and_your_safety.mp3</t>
   </si>
   <si>
@@ -489,51 +580,55 @@
     <t>violence_on_women.png</t>
   </si>
   <si>
+    <t>c2_1_1_violence_on_women.mp3</t>
+  </si>
+  <si>
     <t>violence_on_women.mp3</t>
   </si>
   <si>
     <t>&lt;div&gt;
-  &lt;ul&gt;
+  &lt;ul style='marginLeft: -18;'&gt;
     &lt;li&gt;អំពីហិង្សាលើស្ត្រី គឺជាទង្វើអំពើហិង្សាដែលទាក់ទងនឹងយេនឌ័រដែលនាំឲ្យមាន ឬទំនងជាបង្កអោយមានគ្រោះថ្នាក់ ឬការឈឺចាប់ផ្លូវកាយ ផ្លូវភេទ ឬផ្លូវចិត្តដល់ស្រ្តីរួមនឹងការគំរាមកំហែងប្រព្រឹត្តទង្វើទំាងនេះ ការបង្ខិតបង្ខំ ការបំបិទសេរីភាពតាមអំពើចិត្តមិនថាកើតមានឡើងនៅទីសាធារណៈ ឬ ជីវិតឯកជននោះទេ។&lt;/li&gt;
     &lt;li&gt;អំពីហិង្សាលើស្ត្រីគ្រប់ទម្រង់ គឺជាការរំលោភសិទ្ធិស្រ្តី។&lt;/li&gt;
   &lt;/ul&gt;
-  &lt;h2&gt;ទម្រង់ផ្សេងៗអំពើហិង្សាលើស្រ្តី&lt;/h2&gt;
-  &lt;div style='display: flex; flex-direction: row'&gt;
-    &lt;div style='width: 130px;'&gt;ហិង្សាផ្លូវកាយ៖&lt;/div&gt;&lt;div style='flex: 1'&gt;វាយដំ ឬដាល់ រុញឲ្យដួល ទះ តប់ គប់ដោយប្រើរបស់ផ្សេងៗ ការខំា ការទាញសក់ ការកាត់ ឬចាក់ ការធ្វើអោយថប់ដង្ហើម និងការដុត ។ល។&lt;/div&gt;
-  &lt;/div&gt;
-  &lt;div style='display: flex; flex-direction: row'&gt;
+  &lt;h2 style='marginBottom: 10;'&gt;ទម្រង់ផ្សេងៗអំពើហិង្សាលើស្រ្តី&lt;/h2&gt;
+  &lt;div&gt;
+    &lt;div&gt;ហិង្សាផ្លូវកាយ៖&lt;/div&gt;
+    &lt;div style='marginLeft: 20;'&gt;វាយដំ ឬដាល់ រុញឲ្យដួល ទះ តប់ គប់ដោយប្រើរបស់ផ្សេងៗ ការខំា ការទាញសក់ ការកាត់ ឬចាក់ ការធ្វើអោយថប់ដង្ហើម និងការដុត ។ល។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex;'&gt;
     &lt;div style='width: 130px;'&gt;ហិង្សាផ្លូវចិត្ត៖&lt;/div&gt;
-    &lt;div style='flex: 1'&gt;
-      &lt;ul style='marginTop: 0;'&gt;
-        &lt;li&gt;ជេរប្រមាថ មើលងាយ ឬសម្លុតគំរាមកំហែង&lt;/li&gt;
-        &lt;li&gt;មិនគោរព ផ្តល់តម្លៃ និងទំនុកចិត្ត&lt;/li&gt;
-        &lt;li&gt;និយាយចំអកបញ្ឈឺចិត្ត និងធ្វើអោយអាម៉ាសមុខ&lt;/li&gt;
-        &lt;li&gt;ការបដិសេដលើគំនិត និងយោបល់&lt;/li&gt;
-        &lt;li&gt;គ្រប់គ្រង និងបំបិតសិទ្ធសេរីភាព&lt;/li&gt;
+    &lt;div style='marginLeft: 20;'&gt;
+      &lt;ul style='marginTop: 0; marginLeft: -18;'&gt;
+        &lt;li&gt;ជេរ​ប្រមាថ​ មើល​ងាយ​ ឬ​សម្លុត​គំរាម​កំហែង&lt;/li&gt;
+        &lt;li&gt;មិន​គោរព​ ផ្តល់​តម្លៃ​ និង​ទំនុក​ចិត្ត&lt;/li&gt;
+        &lt;li&gt;និយាយ​ចំអក​បញ្ឈឺ​ចិត្ត​ និង​ធ្វើ​អោយ​អាម៉ាសមុខ&lt;/li&gt;
+        &lt;li&gt;ការ​បដិសេដ​លើ​គំនិត​ និង​យោបល់&lt;/li&gt;
+        &lt;li&gt;គ្រប់​គ្រង​ និង​បំបិត​សិទ្ធ​សេរីភាព&lt;/li&gt;
         &lt;li&gt;បដិសេធមិនគោរពនូវជំនឿ&lt;/li&gt;
         &lt;li&gt;ការរំពឹងចង់បានច្រើនហួសហេតុ&lt;/li&gt;
         &lt;li&gt;ចេះតែរិះគន់ឥតឈប់ឈរ&lt;/li&gt;
-        &lt;li&gt;ទាមទារអ្វីៗដោយមិនសមហេតុផល&lt;/li&gt;
-        &lt;li&gt;និយាយចោទប្រកាន់ ស្តីបន្ទោស គំរាម ឬបង្គាប់បញ្ជា&lt;/li&gt;
+        &lt;li&gt;ទាម​ទារ​អ្វីៗ​ដោយ​មិន​សម​ហេតុផល&lt;/li&gt;
+        &lt;li&gt;និយាយ​ចោទ​ប្រកាន់​ ស្តី​បន្ទោស​ គំរាម​ ឬ​បង្គាប់​បញ្ជា&lt;/li&gt;
       &lt;/ul&gt;
     &lt;/div&gt;
   &lt;/div&gt;
-  &lt;div style='display: flex; flex-direction: row'&gt;
+  &lt;div style='display: flex; marginTop: -20'&gt;
     &lt;div style='width: 130px;'&gt;ហិង្សាផ្លូវភេទ៖&lt;/div&gt;
-    &lt;div style='flex: 1'&gt;ការរំលោភសេពសន្ថវៈ, ការរំលោភសេពសន្ថវៈក្នុងចំណងអាពាហ៍ពិពាហ៍, ស្មន្ធការ (ការរួមភេទជាមួយសាច់ញាតិខ្លួនឯង), បៀតបៀនផ្លូវភេទ, រុកគួនខាងផ្លូវភេទ, បង្ហាញកេរភេទ, ការនិយាយទាក់ទងផ្លូវភេទដែលមិនសមរម្យ ឬសំដែងឥរិយាបទផ្លូវភេទដែលធ្វើឲ្យមានការភ័យខ្លាច, ការប៉ះពាល់រាងកាយ ឬកេរិ៍្តភេទដោយចេតនា, ការបង្ខំឲ្យធ្វើសកម្មភាពផ្លូវភេទ ដូចជាបង្ខំឲ្យរួមភេទតាមមាត់, មើលរឿងអាសអាភាស, ផលិតសម្ភារៈ ឬឧបករណ៍អាសអាភាស ឬមើលសកម្មភាពរួមភេទ ឬលើកទឹកចិត្តអោយប្រព្រឹត្តអាកប្បកិរិយាទាក់ទងនឹងផ្លូវភេទមិនសមរម្យ។ល។&lt;/div&gt;
-  &lt;/div&gt;
-  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='marginLeft: 20;'&gt;ការរំលោភសេពសន្ថវៈ, ការរំលោភសេពសន្ថវៈក្នុងចំណងអាពាហ៍ពិពាហ៍, ស្មន្ធការ (ការរួមភេទជាមួយសាច់ញាតិខ្លួនឯង), បៀតបៀនផ្លូវភេទ, រុកគួនខាងផ្លូវភេទ, បង្ហាញកេរភេទ, ការនិយាយទាក់ទងផ្លូវភេទដែលមិនសមរម្យ ឬសំដែងឥរិយាបទផ្លូវភេទដែលធ្វើឲ្យមានការភ័យខ្លាច, ការប៉ះពាល់រាងកាយ ឬកេរិ៍្តភេទដោយចេតនា, ការបង្ខំឲ្យធ្វើសកម្មភាពផ្លូវភេទ ដូចជាបង្ខំឲ្យរួមភេទតាមមាត់, មើលរឿងអាសអាភាស, ផលិតសម្ភារៈ ឬឧបករណ៍អាសអាភាស ឬមើលសកម្មភាពរួមភេទ ឬលើកទឹកចិត្តអោយប្រព្រឹត្តអាកប្បកិរិយាទាក់ទងនឹងផ្លូវភេទមិនសមរម្យ។ល។&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex;'&gt;
     &lt;div style='width: 130px;'&gt;ហិង្សាផ្នែកសេដ្ឋកិច្ច៖&lt;/div&gt;
-    &lt;div style='flex: 1'&gt;មិនអនុញ្ញាតឱ្យទទួលបានអាហារ ប្រាក់កាស សម្លៀកបំពាក់ ថ្នាំសង្កូវ ការអប់រំ មិនអនុញ្ញាតឱ្យទៅធ្វើការងារ បង្ខំឱ្យធ្វើការងារ ដកហូតប្រាក់ចំនូលទាំងអស់ ពុំផ្តល់សិទ្ធិកាន់កាប់ទ្រព្យសម្បត្តិ&lt;/div&gt;
-  &lt;/div&gt;
-  &lt;div style='display: flex; flex-direction: row'&gt;
-    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ខ្ញុំបានឮថាបងប្អូនស្រ្តីពលករចំណាកស្រុកជួបនូវបទពិសោធអំពើហិង្សា តើកុលាបមានដែលឭ ឬឃើញអំពីហិង្សាលើស្រ្តីទេ?&lt;/div&gt;
-  &lt;/div&gt;
-  &lt;div style='display: flex; flex-direction: row'&gt;
-    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ខ្ញុំបានដឹងរឿងមិត្តរួមការងារជិតស្និតម្នាក់ គឺរស្មី។ រស្មីគាត់រៀបការប្រមាណជាង៣ឆ្នាំហើយ ​ជាមួយនឹងប្តី របស់គាត់ឈ្មោះវិច្ឆិកា ដែលធ្វើការនៅថៃទាំងពីរនាក់។ រស្មីប្រាប់ខ្ញុំថា មុនរៀបការ វិច្ឆិកា គឺប្រចណ្ទ័ខ្លាំងណាស់។ តែពេលណុង៎ រស្មីគិតថាដោយសារតែគាត់ស្រលាញ់នាងខ្លាំងពេក។ ដល់ពេលរៀបការហើយ ប្តីរបស់រស្មី គឺមិនចង់ឲ្យគាត់រាប់អានមិត្តភក្តិ ឬធ្វើការកន្លែងបែកពីគ្នាទេ។ ប៉ុន្តែប្តីរបស់រស្មីវិញ ឲ្យតែបើកប្រាក់ខែម្តងៗ ដឹងតែដើរលេងជាមួយនិងគូរកនរបស់គេដាច់យប់រហូត។ រស្មីបានប្រាប់ខ្ញុំទៀតថា ពេលមួយនោះ ក្រោយពីបើកប្រាក់ខែហើយ ប្តីគេដើរសប្បាយដល់យប់ជ្រៅ ស្រាប់តែមកដល់ផ្ទះរករឿង ថារស្មីមានប្រុសអីណា​ ដោយគ្មានហេតុផលអីសោះ ដល់ពេលនាងប្រកែក ប្តីនាងបានទះកំផ្លៀង និងរុញឲ្យដួល។​ ក្រោយមក វិច្ឆិកាបានមកសុំទោសដែលបានជ្រុលដៃទះកំផ្លៀងប្រពន្ធ និងសន្យាមិនធ្វើអញ្ចឹងទៀតទេ។ មិនបានប្រហែលមួយអាទិត្យផង ប្តីរស្មីបានធ្វើទង្វើនេះដដែល ហើយកាន់តែអាក្រក់ជាងមុនទៅទៀត គឺបានដាល់មុខរស្មីមួយដៃយ៉ាងធ្ងន់។ &lt;/div&gt;
-  &lt;/div&gt;
-  &lt;div style='display: flex; flex-direction: row'&gt;
-    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ដល់ថ្នាក់ហ្នឹងផង! វិច្ឆកានោះពិតជាអាក្រក់មែន គេគួរតែត្រូវបានទទួលទោសចំពោះទង្វើហិង្សាដែលគេបានប្រព្រឹត្តិមកលើរស្មី។ តែជាការល្អណាស់ ដែលរស្មីមានមិត្តល្អដូចកុលាបឯង ព្រោះនាងមាន មិត្តល្អដែលអាចទុកចិត្តនិយាយរឿងរ៉ាវក្នុងចិត្តប្រាប់បាន។&lt;/div&gt;
+    &lt;div style='marginLeft: 20;'&gt;មិនអនុញ្ញាតឱ្យទទួលបានអាហារ ប្រាក់កាស សម្លៀកបំពាក់ ថ្នាំសង្កូវ ការអប់រំ មិនអនុញ្ញាតឱ្យទៅធ្វើការងារ បង្ខំឱ្យធ្វើការងារ ដកហូតប្រាក់ចំនូលទាំងអស់ ពុំផ្តល់សិទ្ធិកាន់កាប់ទ្រព្យសម្បត្តិ&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row; marginTop: 30'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ខ្ញុំ​បាន​ឮ​ថា​បង​ប្អូន​ស្រ្តី​ពលករ​ចំណាក​ស្រុក​ជួប​នូវ​បទពិសោធន៍​អំពើ​ហិង្សា​ តើ​កុលាប​មាន​ដែល​ឭ​ ឬ​ឃើញ​អំពី​ហិង្សា​លើ​ស្រ្តី​ទេ?&lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;កុលាប៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ខ្ញុំ​បាន​ដឹង​រឿង​មិត្ត​រួម​ការ​ងារ​ជិត​ស្និត​ម្នាក់​ គឺ​រស្មី។​ រស្មី​គាត់​រៀប​ការ​ប្រមាណ​ជាង​៣ឆ្នាំ​ហើយ​ ​ជា​មួយ​នឹង​ប្តី​ របស់​គាត់ឈ្មោះ​វិច្ឆិកា​ ដែល​ធ្វើ​ការ​នៅ​ថៃ​ទាំង​ពីរ​នាក់។​ រស្មី​ប្រាប់​ខ្ញុំ​ថា​ មុន​រៀប​ការ​ វិច្ឆិកា​ គឺ​ប្រចណ្ទ័​ខ្លាំង​ណាស់។​ តែ​ពេល​ណុង៎​ រស្មី​គិត​ថា​ដោយ​សារ​តែ​គាត់​ស្រលាញ់​នាង​ខ្លាំង​ពេក។​ ដល់​ពេល​រៀប​ការ​ហើយ​ ប្តី​របស់​រស្មី​ គឺ​មិន​ចង់​ឲ្យ​គាត់​រាប់​អាន​មិត្ត​ភក្តិ​ ឬ​ធ្វើ​ការ​កន្លែង​បែក​ពី​គ្នា​ទេ។​ ប៉ុន្តែ​ប្តី​របស់​រស្មី​វិញ​ ឲ្យ​តែ​បើក​ប្រាក់​ខែ​ម្តងៗ​ ដឹង​តែ​ដើរ​លេង​ជា​មួយ​និង​គូរ​កន​របស់​គេ​ដាច់​យប់​រហូត។​ រស្មី​បាន​ប្រាប់ខ្ញុំ​ទៀត​ថា​ ពេល​មួយ​នោះ​ ក្រោយ​ពី​បើក​ប្រាក់​ខែ​ហើយ​ ប្តី​គេ​ដើរ​សប្បាយ​ដល់​យប់​ជ្រៅ​ ស្រាប់​តែ​មក​ដល់​ផ្ទះ​រក​រឿង​ ថា​រស្មី​មាន​ប្រុស​អី​ណា​ ដោយ​គ្មាន​ហេតុ​ផល​អីសោះ​ ដល់​ពេល​នាង​ប្រកែក​ ប្តី​នាង​បាន​ទះ​កំផ្លៀង​ និង​រុញ​ឲ្យ​ដួល។​​ ក្រោយ​មក​ វិច្ឆិកា​បាន​មក​សុំ​ទោស​ដែល​បាន​ជ្រុល​ដៃ​ទះ​កំផ្លៀង​ប្រពន្ធ​ និង​សន្យា​មិន​ធ្វើ​អញ្ចឹង​ទៀត​ទេ។​ មិន​បាន​ប្រហែល​មួយ​អាទិត្យ​ផង​ ប្តី​រស្មី​បាន​ធ្វើ​ទង្វើ​នេះ​ដដែល​ ហើយ​កាន់​តែ​អាក្រក់​ជាង​មុន​ទៅ​ទៀត​ គឺ​បាន​ដាល់​មុខ​រស្មី​មួយ​ដៃ​យ៉ាង​ធ្ងន់។​ &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div style='display: flex; flex-direction: row'&gt;
+    &lt;div style='width: 90px;'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ដល់​ថ្នាក់​ហ្នឹង​ផង!​ វិច្ឆកា​នោះ​ពិត​ជា​អាក្រក់​មែន​ គេ​គួរ​តែ​ត្រូវ​បាន​ទទួល​ទោស​ចំពោះ​ទង្វើ​ហិង្សា​ដែល​គេ​បាន​ប្រព្រឹត្តិ​មក​លើ​រស្មី។​ តែ​ជា​ការ​ល្អ​ណាស់​ ដែល​រស្មី​មាន​មិត្ត​ល្អ​ដូច​កុលាប​ឯង​ ព្រោះ​នាង​មាន​ មិត្ត​ល្អ​ដែល​អាច​ទុក​ចិត្ត​និយាយ​រឿង​រ៉ាវ​ក្នុង​ចិត្ត​ប្រាប់​បាន។​&lt;/div&gt;
   &lt;/div&gt;
 &lt;/div&gt;</t>
   </si>
@@ -545,6 +640,9 @@
   </si>
   <si>
     <t>harassment.png</t>
+  </si>
+  <si>
+    <t>c2_1_2_harassment.mp3</t>
   </si>
   <si>
     <t>harassment.mp3</t>
@@ -554,21 +652,21 @@
   &lt;div&gt;ការបៀតបៀនផ្លូវភេទ គឺជាទង្វើ ឬឥរិយាបថទាំងឡាយណាដែលមិនចង់បាន មិនស្វាគមន៍ ឬក៏មិនអនុញ្ញាតពាក់ព័ន្ធនឹងផ្លូវភេទដែលធ្វើអោយបុគ្គលម្នាក់ ឬច្រើននាក់មានអារម្មណ៍អាម៉ាស់មុខ ភិតភ័យ ឬអាក់អន់ចិត្ដ។ ការបៀតបៀនផ្លូវភេទមានទម្រង់ខុសគ្នារួមមាន៖ ការបៀតបៀនផ្លូវភេទដោយប្រើអំណាច ពាក្យសម្ដី សំលេង និងការបៀតបៀនផ្លូវភេទដោយកាយវិការ ។&lt;/div&gt;
   &lt;div style='color: red; margin-top: 10px'&gt;ឧទាហរណ៍ ការបៀតបៀនផ្លូវភេទដោយពាក្យសម្ដី&lt;/div&gt;
   &lt;ul&gt;
-    &lt;li&gt;ការប្រើប្រាស់ភាសាមិនសមរម្យ ឬភាសាអាសអាភាស និងនិយាយលេងសើចបែបអាសអាភាស&lt;/li&gt;
-    &lt;li&gt;ការហៅមិនសមរម្យទៅកាន់ស្រ្ដីនៅតាមផ្លូវ ឬការប្រើភាសាអាសអាភាសនៅពេលស្រ្តីដើរកាត់&lt;/li&gt;
-    &lt;li&gt;ការហូចបែបមិនសមរម្យនៅពេលស្រ្តីដើរកាត់&lt;/li&gt;
-    &lt;li&gt;សំណើរ និងការលួងលោមដដែលៗ ដើម្បីបំពេញចំណង់ផ្លូវភេទ ឬការណាត់ជួបក្នុងគោលបំណងផ្លូវភេទ&lt;/li&gt;
-    &lt;li&gt;ការនិយាយសម្តីដែលមានលក្ខណៈផ្លូវភេទ (ឧទាហរណ៍៖ ហៅឈ្មោះជាលក្ខណៈផ្លូវភេទ ឬសួរអំពីអត្តសញ្ញាណផ្លូវភេទ ឬការប្រព្រឹត្តខាងផ្លូវភេទ)&lt;/li&gt;
+    &lt;li&gt;ការ​ប្រើ​ប្រាស់​ភាសា​មិន​សមរម្យ​ ឬ​ភាសា​អាសអាភាស​ និង​និយាយ​លេង​សើច​បែប​អាសអាភាស&lt;/li&gt;
+    &lt;li&gt;ការ​ហៅ​មិន​សមរម្យ​ទៅ​កាន់​ស្រ្ដី​នៅ​តាម​ផ្លូវ​ ឬ​ការ​ប្រើ​ភាសា​អាសអាភាស​នៅ​ពេល​ស្រ្តី​ដើរ​កាត់&lt;/li&gt;
+    &lt;li&gt;ការ​ហូច​បែប​មិន​សមរម្យ​នៅ​ពេល​ស្រ្តី​ដើរ​កាត់&lt;/li&gt;
+    &lt;li&gt;សំណើរ​ និង​ការ​លួង​លោម​ដដែលៗ​ ដើម្បី​បំពេញ​ចំណង់​ផ្លូវ​ភេទ​ ឬ​ការ​ណាត់​ជួប​ក្នុង​គោល​បំណង​ផ្លូវ​ភេទ&lt;/li&gt;
+    &lt;li&gt;ការ​និយាយ​សម្តី​ដែល​មាន​លក្ខណៈ​ផ្លូវ​ភេទ​ (ឧទាហរណ៍៖​ ហៅឈ្មោះ​ជា​លក្ខណៈ​ផ្លូវ​ភេទ​ ឬ​សួរ​អំពី​អត្ត​សញ្ញាណ​ផ្លូវ​ភេទ​ ឬ​ការ​ប្រព្រឹត្ត​ខាង​ផ្លូវ​ភេទ)&lt;/li&gt;
     &lt;li&gt;ការវាយប្រហារឯកជនភាព ទាំងក្នុង និងក្រៅសាលារៀន ឬកន្លែងធ្វើការ (ឧទាហរណ៍៖ការបៀតបៀន ដោយការហៅទៅទូរស័ព្ទ ឬដើរតាមស្រ្ដីនោះដល់ផ្ទះ)&lt;/li&gt;
-    &lt;li&gt;ការស្នើដាក់លក្ខខណ្ឌដោះដូរដើម្បីបំពេញចំណង់ផ្លូវភេទផ្ទាល់ខ្លួន ដូចជា ការផ្ទេរ ការដំឡើងឋានៈ ប្រាក់ខែ ឬបន្ដការងារ&lt;/li&gt;
-    &lt;li&gt;គំរាមកំហែងវាយធ្វើបាប បង្ខិតបង្ខំ ឬរំលោភផ្លូវភេទ។&lt;/li&gt;
+    &lt;li&gt;ការ​ស្នើ​ដាក់លក្ខខណ្ឌ​ដោះ​ដូរ​ដើម្បី​បំពេញ​ចំណង់​ផ្លូវ​ភេទ​ផ្ទាល់​ខ្លួន​ ដូច​ជា​ ការ​ផ្ទេរ​ ការ​ដំឡើង​ឋានៈ​ ប្រាក់​ខែ​ ឬ​បន្ដ​ការងារ&lt;/li&gt;
+    &lt;li&gt;គំរាម​កំហែង​វាយ​ធ្វើ​បាប​ បង្ខិត​បង្ខំ​ ឬ​រំលោភ​ផ្លូវ​ភេទ។&lt;/li&gt;
   &lt;/ul&gt;
   &lt;div style='color: red;'&gt;ឧទាហរណ៍ ការបៀតបៀនផ្លូវភេទដោយកាយវិការ&lt;/div&gt;
   &lt;ul&gt;
-    &lt;li&gt;ការតាំងបង្ហាញវត្ថុដែលធ្វើឱ្យនឹកឃើញដល់ផ្លូវភេទ ដូចជារូបភាព ទស្សនាវដ្ដី ផ្ទាំងរូបភាព ឬតុក្កតាអាសអាភាស&lt;/li&gt;
-    &lt;li&gt;ការសម្លក់សម្លឹង ឬសញ្ញាកាយវិការដែលទាក់ទងនឹងផ្លូវភេទ&lt;/li&gt;
-    &lt;li&gt;ការប៉ះ ការថើប ការឱបក្រសោប ការធ្វើសរសៃ ឬការអង្អែលលើរាងកាយដែលមិនអនុញាត&lt;/li&gt;
-    &lt;li&gt;ការវាយធ្វើបាប ឬបង្ខិតបង្ខំ និងរំលោភផ្លូវភេទ &lt;/li&gt;
+    &lt;li&gt;ការ​តាំង​បង្ហាញ​វត្ថុ​ដែល​ធ្វើ​ឱ្យ​នឹក​ឃើញ​ដល់​ផ្លូវ​ភេទ​ ដូច​ជា​រូបភាព​ ទស្សនាវដ្ដី​ ផ្ទាំង​រូបភាព​ ឬ​តុក្កតា​អាសអាភាស&lt;/li&gt;
+    &lt;li&gt;ការ​សម្លក់​សម្លឹង​ ឬ​សញ្ញា​កាយ​វិការ​ដែល​ទាក់​ទង​នឹង​ផ្លូវ​ភេទ&lt;/li&gt;
+    &lt;li&gt;ការ​ប៉ះ​ ការ​ថើប​ ការ​ឱប​ក្រសោប​ ការ​ធ្វើ​សរសៃ​ ឬ​ការ​អង្អែល​លើ​រាង​កាយ​ដែល​មិន​អនុញាត&lt;/li&gt;
+    &lt;li&gt;ការ​វាយ​ធ្វើ​បាប​ ឬ​បង្ខិត​បង្ខំ​ និង​រំលោភ​ផ្លូវ​ភេទ &lt;/li&gt;
   &lt;/ul&gt;
   &lt;div&gt;ទោះបីជានរណាក៏អាចជាកម្មវត្ថុនៃអំពើបៀតបៀនផ្លូវភេទ ស្រ្តីភាគច្រើនត្រូវបានក្លាយជាជនរងគ្រោះនៃការបៀតបៀនផ្លូវភេទ។ ទម្រង់នៃការការបៀតបៀនផ្លូវភេទ គឺអាចកើតមាននៅគ្រប់ទីកន្លែងទាំងអស់ រួមទាំងកន្លែងធ្វើការ។ នៅកន្លែងធ្វើការ ការបៀតបៀនផ្លូវភេទពេលខ្លះ គឺជាទង្វើមួយដែលជម្រុញឲ្យទទួលយកជាថ្នូរ និងផលប្រយោជន៍ត្រលប់មកវិញ។ ជាក់ស្តែង ការស្នើដាក់លក្ខខណ្ឌដោះដូរដើម្បីបំពេញចំណង់ផ្លូវភេទផ្ទាល់ខ្លួន ដូចជា ការផ្ទេរ ការដំឡើងឋានៈ ប្រាក់ខែ ឬបន្ដការងារ។&lt;/div&gt;
 &lt;/div&gt;</t>
@@ -583,20 +681,23 @@
     <t>your_health.png</t>
   </si>
   <si>
+    <t>c2_1_3_your_health.mp3</t>
+  </si>
+  <si>
     <t>your_health.mp3</t>
   </si>
   <si>
     <t>&lt;div&gt;
-  &lt;div&gt;ការថែទាំសុខភាពរបស់អ្នក គឺមានសារៈសំខាន់ណាស់ ទន្ទឹមនឹងពេលដែលអ្នកខ្វល់ខ្វាយ និងរវល់ជាមួយការងារប្រចាំថ្ងៃ។ &lt;/div&gt;
+  &lt;div&gt;ការ​ថែទាំ​សុខភាព​របស់​អ្នក​ គឺ​មាន​សារៈ​សំខាន់​ណាស់​ ទន្ទឹម​នឹង​ពេល​ដែល​អ្នក​ខ្វល់​ខ្វាយ​ និង​រវល់​ជា​មួយ​ការងារ​ប្រចាំ​ថ្ងៃ។ &lt;/div&gt;
   &lt;ul&gt;
-    &lt;li&gt;មិនមែនជាការខ្មាស់អៀននោះទេក្នុងការនិយាយអំពីបទពិសោធ ឬចំងល់ផ្សេងៗទាក់ទងនឹងការមករដូវរបស់អ្នក។ មិត្តភក្តិជិតស្និទ្ធ ឬបងប្អូនស្រី ឬម្តាយអាចជាមនុស្សដែលគួរឲ្យទុកចិត្ត និងមានអារម្មណ៍សុវត្ថិភាពសម្រាប់អ្នកក្នុងការនិយាយប្រាប់អំពីកង្វល់ ឬការព្រួយបារម្ភផ្សេងៗអំពីការមករដូវរបស់អ្នក។&lt;/li&gt;
+    &lt;li&gt;មិន​មែន​ជា​ការ​ខ្មាស់​អៀន​នោះ​ទេ​ក្នុង​ការ​និយាយ​អំពី​បទពិសោធន៍​ ឬ​ចំងល់​ផ្សេងៗ​ទាក់ទង​នឹង​ការ​មក​រដូវ​របស់​អ្នក។​ មិត្ត​ភក្តិ​ជិត​ស្និទ្ធ​ ឬ​បង​ប្អូន​ស្រី​ ឬ​ម្តាយ​អាច​ជា​មនុស្ស​ដែល​គួរ​ឲ្យ​ទុក​ចិត្ត​ និង​មាន​អារម្មណ៍​សុវត្ថិភាព​សម្រាប់​អ្នក​ក្នុង​ការ​និយាយ​ប្រាប់​អំពី​កង្វល់​ ឬ​ការ​ព្រួយ​បារម្ភ​ផ្សេងៗ​អំពី​ការ​មក​រដូវ​របស់​អ្នក។&lt;/li&gt;
     &lt;li&gt;ជាធម្មតា ស្រ្តីមករដូវជារៀងរាល់ចន្លោះពី ២៨ ទៅ ៤០ ថ្ងៃ ដែលជាវដ្តទូទៅ ហើយជារឿងធម្មតា។ រដូវ ទៀង គឺមានន័យថាមកជារៀងរាល់ ២៨ ថ្ងៃម្តង។ ប៉ុន្តែជាករណីកម្រដែលស្រ្តីមករដូវទៀងក្នុងកំឡុងពេល ២៨ថ្ងៃ។ ស្រ្តីខ្លះអាចមករដូវក្នុងកំឡុងពេល ៣០ ថ្ងៃ អ្នកខ្លះ ៣១ ថ្ងៃ ឬអ្នកខ្លះ ៣៥ ថ្ងៃ លើសពីនេះទៀតមានអ្នកខ្លះរហូតដល់ ៤០ ថ្ងៃ។&lt;/li&gt;
-    &lt;li&gt;យុវតី និងស្រ្តីមានការព្រួយបារម្ភពីការធ្លាក់សរបស់ពួកគេ។ ជាធម្មតា ស្រ្តីមានការធ្លាក់សមុនមករដូវ និងក្រោយមករដូវ។ នេះជារឿងធម្មតាទេ។ ប៉ុន្តែ ប្រសិនបើការធ្លាក់ស របស់អ្នកមានធុំក្លិន មានពណ៌ដូចជាសំបោរពណ៌លឿង អ្នកគួរតែរកការពិគ្រោះយោបល់ជាមួយគ្រូពេទ្យខាងផ្នែករោគស្រ្តី។ &lt;/li&gt;
-    &lt;li&gt;អនាម័យនៅពេលមានរដូវ ដូចជាការលាងសម្អាតឲ្យបានញឹកញាប់ ការប្តូរសំឡីអនាម័យ ឬក្រណាត់ទ្រាប់ ជារៀងរាល់ ៣ ទៅ ៤ ម៉ោង ការហូបអាហារមានបន្លែ ផ្លែឈើ និងហូបទឹកឲ្យបានច្រើន សម្រាកឲ្យបានគ្រប់គ្រាន់ គឺជួយនាំមកនូវសុខភាពបន្តពូជល្អ និងរឹងមាំ។&lt;/li&gt;
-    &lt;li&gt;ការស្វែងរកការពិគ្រោះយោបល់ជាមួយគ្រូពេទ្យខាងផ្នែករោគស្រ្តី គឺមានសារៈសំខាន់ណាស់។ កុំភ្លេចណា៎ ការនិយាយពីការមករដូវ ឬសុខភាពបន្តពូជ មិនមែនជារឿងខ្មាស់អៀនទេ!!!&lt;/li&gt;
-    &lt;li&gt;អ្នក គឺជាម្ចាស់លើរាងកាយរបស់អ្នក។ អ្នកមានសិទ្ធិធ្វើសេចក្តីសម្រេចចិត្តលើផែនការពន្យារកំណើត និងការកំណត់ចំនួនកូនដែលអ្នកចង់បាន។ មានជម្រើសជាច្រើន ដូចជា ការប្រើប្រាស់ស្រោមអនាម័យ ថ្នាំចាក់ ថ្នាំគ្រាប់ កងដាក់ក្រោមស្បែក និងកងដាក់ក្នុងស្បូន ដែលជាសេវាសុខភាពសាធារណៈ ហើយអាចរកសេវានេះបាន ដូចជា មណ្ឌលសុខភាព ឬមន្ទីរពេទ្យបង្អែកជាដើម ដែលជាមធ្យោបាយមានប្រសិទ្ធិភាពខ្ពស់សម្រាប់ការពន្យាកំណើត។ មធ្យោបាយពន្យាកំណើតបែបធម្មជាតិ ដូចជាតាមរយៈការបំបៅដោះកូន តាមរយៈប្រតិទិន តាមរយៈការដកទឹកកាមចេញ។ ប្រសិទ្ធភាពរបស់វា គឺមិនមានខ្ពស់ទេ ហើយប្រឈមនឹងមានផ្ទៃពោះដោយមិនចង់បាន ឬចៃដន្យ។ &lt;/li&gt;
+    &lt;li&gt;យុវតី​ និង​ស្រ្តី​មាន​ការ​ព្រួយ​បារម្ភ​ពី​ការ​ធ្លាក់ស​របស់​ពួក​គេ។​ ជា​ធម្មតា​ ស្រ្តី​មាន​ការ​ធ្លាក់ស​មុន​មក​រដូវ​ និង​ក្រោយ​មក​រដូវ។​ នេះ​ជា​រឿង​ធម្មតា​ទេ។​ ប៉ុន្តែ​ ប្រសិន​បើ​ការ​ធ្លាក់ស​ របស់​អ្នក​មាន​ធុំ​ក្លិន​ មាន​ពណ៌​ដូច​ជា​សំបោរ​ពណ៌​លឿង​ អ្នក​គួរ​តែ​រក​ការ​ពិគ្រោះ​យោបល់​ជា​មួយ​គ្រូពេទ្យ​ខាង​ផ្នែក​រោគ​ស្រ្តី។ &lt;/li&gt;
+    &lt;li&gt;អនាម័យ​នៅ​ពេល​មាន​រដូវ​ ដូច​ជា​​ការ​​លាង​​សម្អាត​​ឲ្យ​​បាន​​ញឹក​ញាប់​​ ការ​​ប្តូរ​​សំឡី​​អនាម័យ​​ ឬ​​ក្រណាត់​ទ្រាប់​ ជា​រៀង​រាល់​ ៣ ទៅ​ ៤ ម៉ោង​ ការ​ហូប​អាហារ​មាន​បន្លែ​ ផ្លែ​ឈើ​ និង​ហូប​ទឹក​ឲ្យ​បាន​ច្រើន​ សម្រាក​ឲ្យ​បាន​គ្រប់​គ្រាន់​ គឺ​ជួយ​នាំ​មក​នូវ​សុខ​ភាព​បន្ត​ពូជ​ល្អ​ និង​រឹងមាំ។&lt;/li&gt;
+    &lt;li&gt;ការ​ស្វែង​រក​ការ​ពិគ្រោះ​យោបល់​ជា​មួយ​គ្រូពេទ្យ​ខាង​ផ្នែក​រោគ​ស្រ្តី​ គឺ​មាន​សារៈ​សំខាន់​ណាស់។​ កុំ​ភ្លេច​ណា៎​ ការ​និយាយ​ពី​ការ​មក​រដូវ​ ឬ​សុខភាព​បន្ត​ពូជ​ មិន​មែន​ជា​រឿង​ខ្មាស់​អៀន​ទេ!!!&lt;/li&gt;
+    &lt;li&gt;អ្នក​ គឺ​ជា​ម្ចាស់​លើ​រាង​កាយ​របស់​អ្នក។​ អ្នក​មាន​សិទ្ធិ​ធ្វើ​សេចក្តី​សម្រេច​ចិត្ត​លើ​ផែនការ​ពន្យារ​កំណើត​ និង​ការ​កំណត់​ចំនួន​កូន​ដែល​អ្នក​ចង់​បាន។​ មាន​ជម្រើស​ជា​ច្រើន​ ដូច​ជា​ ការ​ប្រើ​ប្រាស់​ស្រោម​អនាម័យ​ ថ្នាំ​ចាក់​ ថ្នាំ​គ្រាប់​ កង​ដាក់​ក្រោម​ស្បែក​ និង​កង​ដាក់​ក្នុង​ស្បូន​ ដែល​ជា​សេវា​សុខភាព​សាធារណៈ​ ហើយ​អាច​រក​សេវា​នេះ​បាន​ ដូច​ជា​ មណ្ឌល​សុខភាព​ ឬ​មន្ទីរពេទ្យ​បង្អែក​ជាដើម​ ដែល​ជា​មធ្យោបាយ​មាន​ប្រសិទ្ធិភាព​ខ្ពស់​សម្រាប់​ការ​ពន្យា​កំណើត។​ មធ្យោបាយ​ពន្យា​កំណើត​បែប​ធម្មជាតិ​ ដូច​ជា​តាម​រយៈ​ការ​បំបៅ​ដោះ​កូន​ តាម​រយៈ​ប្រតិទិន​ តាម​រយៈ​ការ​ដក​ទឹកកាម​ចេញ។​ ប្រសិទ្ធភាព​របស់​វា​ គឺ​មិន​មានខ្ពស់ទេ ហើយ​ប្រឈម​នឹង​មាន​ផ្ទៃ​ពោះ​ដោយ​មិន​ចង់​បាន​ ឬ​ចៃដន្យ។ &lt;/li&gt;
   &lt;/ul&gt;
-  &lt;div&gt;កុំភ្លេច ពិគ្រោះយោបល់ជាមួយគ្រូពេទ្យជំនាញ នៅពេលអ្នកចង់ធ្វើផែនការពន្យាកំណើត។ ស្វែងយល់ពីផលប៉ះពាល់ និងប្រសិទ្ធិភាពនៃមធ្យោបាយពន្យារកំណើតនិមួយៗ ជាការចាំបាច់!&lt;/div&gt;
+  &lt;div&gt;កុំ​ភ្លេច​ ពិគ្រោះ​យោបល់​ជា​មួយ​គ្រូពេទ្យ​ជំនាញ​ នៅ​ពេល​អ្នក​ចង់​ធ្វើ​ផែនការ​ពន្យា​កំណើត។​ ស្វែង​យល់​ពី​ផល​ប៉ះពាល់​ និង​ប្រសិទ្ធិភាព​នៃ​មធ្យោបាយ​ពន្យារ​កំណើត​និមួយៗ​ ជា​ការ​ចាំបាច់!&lt;/div&gt;
 &lt;/div&gt;</t>
   </si>
   <si>
@@ -609,17 +710,19 @@
     <t>understand_exploitation_and_human_traficking.png</t>
   </si>
   <si>
+    <t>c2_1_4_understand_exploitation_and_human_traficking.mp3</t>
+  </si>
+  <si>
     <t>understand_exploitation_and_human_traficking.mp3</t>
   </si>
   <si>
     <t>&lt;div&gt;
   &lt;div style='display: flex; flex-direction: row'&gt;
-    &lt;div style='width: 90px'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ខ្ញុំបានឮអ្នកភូមិ មេក្រុម មេភូមិ និយាយអីទេថាបងប្អូនស្រ្តីពលករចំណាកស្រុកប្រយត្ន័ត្រូវគេជូញដូរ។ តើយ៉ាងម៉េចវិញ កុលាប? ក្រែងយើងទៅធ្វើការ ចុះហេតុអី្វបានជា គេអាចជួញដូរ ឬកេងប្រវញ្ច័យើងបានយ៉ាងម៉េចវិញ?&lt;/div&gt;
+    &lt;div style='width: 90px'&gt;ម៉ាលីស៖&lt;/div&gt;&lt;div style='flex: 1'&gt;ខ្ញុំ​បាន​ឮ​អ្នក​ភូមិ​ មេក្រុម​ មេភូមិ​ និយាយ​អី​ទេ​ថា​បង​ប្អូន​ស្រ្តី​ពលករ​ចំណាក​ស្រុក​ប្រយត្ន័​ត្រូវ​គេ​ជូញដូរ។​ តើ​យ៉ាង​ម៉េច​វិញ​ កុលាប?​ ក្រែង​យើង​ទៅ​ធ្វើ​ការ​ ចុះ​ហេតុអី្វ​បាន​ជា​ គេ​អាច​ជួញ​ដូរ​ ឬ​កេង​ប្រវញ្ច័​យើង​បាន​យ៉ាង​ម៉េច​វិញ?​&lt;/div&gt;
   &lt;/div&gt;
   &lt;div style='display: flex; flex-direction: row'&gt;
     &lt;div style='width: 90px'&gt;កុលាប៖&lt;/div&gt;
-    &lt;div style='flex: 1'&gt;
-      ខ្ញុំធ្លាប់បានចូលរួមវគ្គបណ្តុះបណ្តាលទាក់ទងអំពីជួញដូរមនុស្ស និងការកេងប្រវញ្ច័ ខ្ញុំអាចប្រាប់ម៉ាលីសបានណា។
+    &lt;div style='flex: 1'&gt;ខ្ញុំធ្លាប់បានចូលរួមវគ្គបណ្តុះបណ្តាលទាក់ទងអំពីជួញដូរមនុស្ស និងការកេងប្រវញ្ច័ ខ្ញុំអាចប្រាប់ម៉ាលីសបានណា។
       &lt;p&gt;ការជួញដូរមនុស្ស គឺជាការជ្រើសរើស ការដឹកជញ្ជូន ការផ្ទេរ ការឃាត់ទុក ឬការផ្តល់ទីជម្រក តាមមធ្យោបាយគំរាមគំហែង ការប្រើកម្លាំង ទម្រង់ផ្សេងទៀតនៃការបង្ខិតបង្ខំ ការចាប់ ពង្រត់ ការក្លែងបន្លំឯកសារ ការបោកប្រាស់ ការរំលោភបំពានអំណាច ការប្រើតួនាទីរំលោភជនរងគ្រោះ ការឲ្យ ឬទទួលយកកម្រៃ ឬអត្ថប្រយោជន៍ណាមួយដើម្បីសម្រេចបានការព្រមព្រៀងឲ្យមានការត្រួតត្រាលើមនុស្សម្នាក់ទៀត។ ការកេងប្រវ័ញ្ចរួមមាន ការកេងប្រវ័ញ្ចលើពេស្យាកម្មជនដទៃ ឬទម្រង់ផ្សេងៗទៀតនៃការកេងប្រវ័ញ្ចផ្លូវភេទ ពលកម្ម ឬសេវាដោយបង្ខំ ទាសភាព ឬការអនុវត្តន៍ស្រដៀងគ្នានឹង ទាសភាព ទាសករ ឬការដកហូតសរីរាង្គណាមួយ។&lt;/p&gt;
     &lt;/div&gt;
   &lt;/div&gt;
@@ -653,6 +756,24 @@
     <t>your_right_and_safety.png</t>
   </si>
   <si>
+    <t>c2_1_5_your_right_and_protection.mp3</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;
+&lt;div&gt;ស្វែងយល់ពីសិទ្ធិរបស់អ្នក&lt;/div&gt;
+&lt;ul&gt;
+&lt;li&gt;ពលករចំណាកស្រុកជាស្ត្រី ទាំងអ្នកមានឯកសារ និងមិនមានឯកសារ គឺត្រូវបានការពារដោយច្បាប់ជាតិ និងអន្តរជាតិ។ ទោះបីអ្នកមកពីណា ស្ថានភាពនៃការធ្វើចំណាស្រុករបស់អ្នកយ៉ាងណាក៏ដោយ អ្នកមានសិទ្ធិទទួលបាននូវសុវត្ថិភាព។&lt;/li&gt;
+&lt;li&gt;ពលករចំណាកស្រុកជាស្ត្រី មានសិទ្ធិទទួលបានក្នុងការរក្សាទុកនូវឯកសារផ្ទាល់ខ្លួន ដូចជាអត្តសញ្ញាណប័ណ្ណ លិខិតឆ្លងដែន និងឯកសារពាក់ព័ន្ធផ្សេងៗទៀត។ មនុស្សគ្រប់រូបត្រូវតែទទួលបាន ការផ្តល់សេវាសាធារណៈ។ ឧទាហរណ៍ សេវាថែទាំសុខភាព ប្រឹក្សាយោបល់ សេវាផ្លូវច្បាប់ជាដើម ដោយគ្មានឧបសគ្គរារាំង។ &lt;/li&gt;
+&lt;li&gt;ពលករចំណាកស្រុកជាស្ត្រី មានសិទ្ធិរួចផុតពីការបៀតបៀនផ្លូវភេទគ្រប់រូបភាព ដូចមានចែងនៅក្នុងអនុសញ្ញា CEDAW និងច្បាប់នានានៅក្នុងប្រទេសគោលដៅ។ &lt;/li&gt;
+&lt;li&gt;ពលករចំណាកស្រុកជាស្ត្រី មានសិទ្ធិការងាសំខាន់ៗដូចជា កិច្ចសន្យាការងារច្បាស់លាស់ ទទួលបានប្រាក់ឈ្នួលស្មើរគ្នា ក្នុងលក្ខខណ្ឌការងារដូចគ្នា។ &lt;/li&gt;
+&lt;li&gt;ពលករចំណាកស្រុកជាស្ត្រី មានសិទ្ធិទទួលបានសុខភាព និងសុវត្ថិភាពការងារដូចគ្នា។ &lt;/li&gt;
+&lt;li&gt;ពលករចំណាកស្រុកជាស្ត្រី មានសិទ្ធិទទួលបានការឈប់សម្រាកប្រចាំឆ្នាំ ឈប់សម្រាកបុណ្យជាតិ ឈប់សម្រាកពេលសម្រាលកូន ដោយទទួលបានប្រាក់ឈ្នួលជាធម្មតា។ &lt;/li&gt;
+&lt;li&gt;ពលករចំណាកស្រុកជាស្ត្រី មានសិទ្ធិទទួលបានសំណង និងការឈប់សម្រាកពីគ្រោះថ្នាក់ការងារ។ &lt;/li&gt;
+&lt;li&gt;ពលករចំណាកស្រុកជាស្ត្រី មានសិទ្ធិទទួលបានក្នុងការចូលរួមជាសមាជិកសមាគមន៍ ឬសហជីព។&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
     <t>sa_002</t>
   </si>
   <si>
@@ -662,6 +783,9 @@
     <t>safety_planning_tips.png</t>
   </si>
   <si>
+    <t>c2_2_safety_plan.mp3</t>
+  </si>
+  <si>
     <t>my_body_my_choice_safety_planning_tips.mp3</t>
   </si>
   <si>
@@ -672,6 +796,9 @@
   </si>
   <si>
     <t>urgent_leave.png</t>
+  </si>
+  <si>
+    <t>c2_2_1_if_need_to_leave_immediately.mp3</t>
   </si>
   <si>
     <t>&lt;div&gt;
@@ -694,6 +821,9 @@
   </si>
   <si>
     <t>checklist.png</t>
+  </si>
+  <si>
+    <t>c2_2_2_things_to_prepare.mp3</t>
   </si>
   <si>
     <t>&lt;div&gt;
@@ -722,6 +852,9 @@
     <t>thing_need_to_know.png</t>
   </si>
   <si>
+    <t>c2_2_3_things_to_understanding.mp3</t>
+  </si>
+  <si>
     <t>&lt;div&gt;
   &lt;div&gt;អ្វីដែលអ្នកត្រូវដឹងបើអ្នកជាស្រ្តីពលករចំណាកស្រុក&lt;/div&gt;
   &lt;ul&gt;
@@ -743,6 +876,9 @@
     <t>safety_more_strategy.png</t>
   </si>
   <si>
+    <t>c2_2_4_other_safety_strategy.mp3</t>
+  </si>
+  <si>
     <t>&lt;div&gt;
   &lt;div&gt;យុទ្ធសាស្រ្តដើម្បីសុវត្ថិភាពផ្សេងទៀត&lt;/div&gt;
   &lt;ul&gt;
@@ -763,7 +899,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -772,10 +908,6 @@
     <font>
       <b/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
       <name val="Arial"/>
     </font>
     <font>
@@ -790,8 +922,14 @@
     <font>
       <name val="Arial"/>
     </font>
+    <font/>
+    <font>
+      <b/>
+      <name val="Arial"/>
+    </font>
     <font>
       <sz val="12.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -799,7 +937,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -818,6 +956,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE5CD"/>
+        <bgColor rgb="FFFCE5CD"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -825,41 +969,59 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1086,14 +1248,14 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="9.57"/>
-    <col customWidth="1" min="2" max="2" width="35.86"/>
-    <col customWidth="1" min="3" max="3" width="39.57"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
-    <col customWidth="1" min="5" max="5" width="12.43"/>
-    <col customWidth="1" min="6" max="6" width="49.86"/>
-    <col customWidth="1" min="8" max="8" width="28.71"/>
-    <col customWidth="1" min="9" max="9" width="29.14"/>
-    <col customWidth="1" min="10" max="10" width="32.0"/>
+    <col customWidth="1" min="2" max="2" width="23.0"/>
+    <col customWidth="1" min="3" max="3" width="29.43"/>
+    <col customWidth="1" min="4" max="5" width="28.86"/>
+    <col customWidth="1" min="6" max="6" width="12.43"/>
+    <col customWidth="1" min="7" max="7" width="49.86"/>
+    <col customWidth="1" min="9" max="9" width="28.71"/>
+    <col customWidth="1" min="10" max="10" width="29.14"/>
+    <col customWidth="1" min="11" max="12" width="32.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1106,10 +1268,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1124,434 +1286,520 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>45</v>
+        <v>53</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="3"/>
+        <v>59</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>52</v>
+        <v>61</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" ht="36.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>56</v>
+        <v>67</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="G10" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>61</v>
+        <v>73</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
     </row>
     <row r="12" ht="37.5" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>66</v>
+        <v>79</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
     </row>
     <row r="13" ht="108.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>71</v>
+        <v>84</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="3"/>
+        <v>87</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>88</v>
+      </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
     </row>
     <row r="14" ht="51.0" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>76</v>
+        <v>90</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>97</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="E15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="F15" s="3"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>83</v>
+        <v>99</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="16" ht="51.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>87</v>
+        <v>104</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" s="3"/>
+        <v>107</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>108</v>
+      </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>92</v>
+        <v>111</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" s="3"/>
+        <v>113</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>114</v>
+      </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-    </row>
-    <row r="18">
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" ht="35.25" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="G18" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D19" s="3"/>
+        <v>122</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="8" t="b">
+      <c r="G19" s="3"/>
+      <c r="H19" s="12" t="b">
         <v>1</v>
       </c>
-      <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId2"/>
@@ -1574,10 +1822,10 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="9.57"/>
     <col customWidth="1" min="2" max="2" width="36.0"/>
-    <col customWidth="1" min="3" max="3" width="44.86"/>
-    <col customWidth="1" min="4" max="4" width="45.43"/>
-    <col customWidth="1" min="5" max="5" width="12.43"/>
-    <col customWidth="1" min="6" max="6" width="36.71"/>
+    <col customWidth="1" hidden="1" min="3" max="3" width="44.86"/>
+    <col customWidth="1" min="4" max="5" width="45.43"/>
+    <col customWidth="1" min="6" max="6" width="12.43"/>
+    <col customWidth="1" min="7" max="7" width="36.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1590,10 +1838,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1602,232 +1850,273 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" s="3"/>
+        <v>126</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" ht="40.5" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>105</v>
+        <v>129</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>130</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>107</v>
+        <v>131</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>133</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" ht="47.25" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>110</v>
+        <v>135</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G4" s="3"/>
+        <v>137</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" ht="32.25" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>117</v>
+        <v>143</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="G5" s="3"/>
+        <v>145</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" ht="30.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>122</v>
+        <v>148</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>150</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7">
+        <v>151</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" ht="66.75" customHeight="1">
       <c r="A7" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="H7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E8" s="3"/>
+        <v>160</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" ht="33.0" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="G9" s="3"/>
+        <v>165</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" ht="21.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>136</v>
+        <v>168</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>169</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="G10" s="3"/>
+        <v>170</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" ht="21.0" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G11" s="3"/>
+        <v>173</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" ht="24.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="G12" s="3"/>
+        <v>179</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="H12" s="3"/>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D13" s="3"/>
+        <v>184</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="8" t="b">
+      <c r="G13" s="3"/>
+      <c r="H13" s="12" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>